<commit_message>
add comment, update test data
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koushiken/Desktop/Software_Test_Project/STV-Project/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BC93DB2-4A4A-ED44-BF3B-554D04A8F120}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1880" windowWidth="25600" windowHeight="16000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" activeTab="3" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -21,15 +22,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ViewTask!$A$1:$A$10</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -37,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J T</author>
   </authors>
   <commentList>
-    <comment ref="H10" authorId="0">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{DCA326BF-D23A-8941-AD0F-8DD6074573D4}">
       <text>
         <r>
           <rPr>
@@ -80,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="392">
   <si>
     <t>component</t>
   </si>
@@ -869,6 +864,28 @@
     <t>//*[@text='not specified']</t>
   </si>
   <si>
+    <r>
+      <t>//*[@text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']</t>
+    </r>
+  </si>
+  <si>
     <t>Input field</t>
   </si>
   <si>
@@ -905,9 +922,6 @@
     <t>//*[@resource-id='org.dmfs.tasks:id/button_add_one_hour']</t>
   </si>
   <si>
-    <t>//*[@class='android.widget.LinearLayout' and @index='1']</t>
-  </si>
-  <si>
     <t>location_link</t>
   </si>
   <si>
@@ -927,9 +941,6 @@
   </si>
   <si>
     <t>check_list_add_item</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='android:id/text1']</t>
   </si>
   <si>
     <t>URL_link</t>
@@ -1063,29 +1074,6 @@
     <t>folder_setting</t>
   </si>
   <si>
-    <r>
-      <t>//*[@class='android.widget.RelativeLayout' and @index='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${INDEX}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'//*[@resource-id='org.dmfs.tasks:id/btn_settings']</t>
-    </r>
-  </si>
-  <si>
     <t>//*[@resource-id='org.dmfs.tasks:id/synced_task_list_button']</t>
   </si>
   <si>
@@ -1271,9 +1259,6 @@
     <t>status_dropdown</t>
   </si>
   <si>
-    <t>TaskList1.png</t>
-  </si>
-  <si>
     <t>reference</t>
   </si>
   <si>
@@ -1478,15 +1463,98 @@
   </si>
   <si>
     <r>
-      <t>//*[@class='</t>
+      <t>//*[@class='android.widget.TextView' and @text='</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>android.widget.LinearLayout</t>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']//*[@resource-id='android:id/text1']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']//*[@resource-id='android:id/checkbox']</t>
+    </r>
+  </si>
+  <si>
+    <t>//*[@index='11']//*[@class='android.widget.Spinner']</t>
+  </si>
+  <si>
+    <t>//*[@text='needs action']</t>
+  </si>
+  <si>
+    <t>//*[@index='12']//*[@class='android.widget.Spinner']</t>
+  </si>
+  <si>
+    <t>//*[@index='13']//*[@class='android.widget.EditText']</t>
+  </si>
+  <si>
+    <t>time_zone_options</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.LinearLayout']//*[contains(@text, '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
     </r>
     <r>
       <rPr>
@@ -1496,7 +1564,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>' and @index='</t>
+      <t>') and @resource-id='org.dmfs.tasks:id/integer_choice_item_text']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>android.widget.LinearLayout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' and ./android.widget.TextView[@text='</t>
     </r>
     <r>
       <rPr>
@@ -1504,7 +1595,45 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>${INDEX}</t>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']]</t>
+    </r>
+  </si>
+  <si>
+    <t>partial name acceptable</t>
+  </si>
+  <si>
+    <t>//*[@text='Medium priority']</t>
+  </si>
+  <si>
+    <t>//*[@text='Low priority']</t>
+  </si>
+  <si>
+    <t>//*[@text='No priority']</t>
+  </si>
+  <si>
+    <t>search_clear_btn</t>
+  </si>
+  <si>
+    <r>
+      <t>//*/android.widget.FrameLayout/android.widget.RelativeLayout//*[@text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
     </r>
     <r>
       <rPr>
@@ -1518,8 +1647,14 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>//*[@class='android.widget.TextView' and @text='</t>
+    <t>//*[@resource-id='org.dmfs.tasks:id/content']//*[@class='android.widget.LinearLayout' and @index='1']</t>
+  </si>
+  <si>
+    <t>${URL}</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[contains(@text, '</t>
     </r>
     <r>
       <rPr>
@@ -1527,21 +1662,25 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>${NAME}</t>
+      <t>${URL}</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>']</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+      <t>')]</t>
+    </r>
+  </si>
+  <si>
+    <t>partial url</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.RelativeLayout' and @index='</t>
     </r>
     <r>
       <rPr>
@@ -1554,46 +1693,86 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>']//*[@resource-id='android:id/text1']</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${INDEX}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']//*[@resource-id='android:id/checkbox']</t>
-    </r>
-  </si>
-  <si>
-    <t>//*[@index='11']//*[@class='android.widget.Spinner']</t>
+      <t>']//*[@resource-id='org.dmfs.tasks:id/btn_settings']</t>
+    </r>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/action_bar_container']//*[@class='android.widget.ImageButton']</t>
+  </si>
+  <si>
+    <t>TaskList.png</t>
+  </si>
+  <si>
+    <t>QuickAddOptions.png</t>
+  </si>
+  <si>
+    <t>Time.png</t>
+  </si>
+  <si>
+    <t>TimeToggleMode.png</t>
+  </si>
+  <si>
+    <t>TimeOptions.png</t>
+  </si>
+  <si>
+    <t>StatusOptions.png</t>
+  </si>
+  <si>
+    <t>PriorityOptions.png</t>
+  </si>
+  <si>
+    <t>PrivacyOptions.png</t>
+  </si>
+  <si>
+    <t>TimezoneOptions.png</t>
+  </si>
+  <si>
+    <t>ViewTask.png</t>
+  </si>
+  <si>
+    <t>ViewTask2.png</t>
+  </si>
+  <si>
+    <t>ConfirmDeleteTask.png</t>
+  </si>
+  <si>
+    <t>ViewTaskMenu.png</t>
+  </si>
+  <si>
+    <t>ViewTaskMenuSeeAll.png</t>
+  </si>
+  <si>
+    <t>ViewTaskMenuCreateTask.png</t>
+  </si>
+  <si>
+    <t>ListSetting.png</t>
+  </si>
+  <si>
+    <t>DisplayedList.png</t>
+  </si>
+  <si>
+    <t>EnterListName.png</t>
+  </si>
+  <si>
+    <t>ConfirmDeleteList.png</t>
+  </si>
+  <si>
+    <t>Synchronize.png</t>
+  </si>
+  <si>
+    <t>PickColor.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1673,14 +1852,6 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1700,14 +1871,14 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1715,38 +1886,38 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1754,7 +1925,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1764,18 +1935,16 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1831,9 +2000,31 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1844,18 +2035,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1865,14 +2044,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1884,9 +2069,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2199,24 +2382,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
     <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2227,42 +2410,42 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="33" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="33"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="33"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2270,9 +2453,9 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="33"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="35"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -2280,9 +2463,9 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="33"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="35"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -2290,9 +2473,9 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="33"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
@@ -2300,31 +2483,31 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="33"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="35"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="33"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E10" s="33"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -2332,64 +2515,67 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="E11" s="33"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E12" s="34"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E12" s="36"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="43" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="35"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="44"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="E16" s="35"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
         <v>49</v>
       </c>
@@ -2397,281 +2583,283 @@
         <v>72</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E17" s="35"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="35"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="35"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="45"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="33" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="34"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="E22" s="36"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="B25" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E25" s="35"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="B26" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E26" s="35"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E25" s="33"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="B26" s="14" t="s">
+      <c r="B27" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E26" s="33"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="E27" s="34"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="36"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="39"/>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E30" s="35"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" s="35"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="B30" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E30" s="33"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="E31" s="33"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="E32" s="33"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E33" s="34"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E33" s="36"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="39"/>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="E35" s="32" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="33" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E36" s="35"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E37" s="35"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E36" s="33"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="B37" s="11" t="s">
+      <c r="B38" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E37" s="33"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="B38" s="11" t="s">
+      <c r="E38" s="35"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E38" s="33"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="E39" s="33"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="35"/>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E40" s="34"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>278</v>
-      </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E40" s="36"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42"/>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="E42" s="33" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="E43" s="35"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="E44" s="35"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="E42" s="32" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E43" s="33"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E44" s="33"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>325</v>
-      </c>
       <c r="B45" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="E45" s="33"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+      <c r="E45" s="35"/>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
         <v>21</v>
       </c>
@@ -2679,171 +2867,178 @@
         <v>138</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="E46" s="33"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E46" s="35"/>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E47" s="34"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
-        <v>279</v>
-      </c>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E47" s="36"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="39"/>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="E49" s="33" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E50" s="35"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E51" s="35"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="C49" s="7"/>
-      <c r="E49" s="32" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="B52" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E52" s="35"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="E50" s="33"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="B51" s="11" t="s">
+      <c r="B53" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E51" s="33"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
-        <v>329</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="E52" s="33"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>330</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="E53" s="33"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="35"/>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E54" s="34"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="31"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E54" s="36"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="39"/>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E56" s="32" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="E57" s="33"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="E57" s="34"/>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="B58" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="E58" s="35"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B59" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="E58" s="33"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="C59" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="E59" s="35"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E59" s="33"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="B60" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E60" s="35"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E60" s="33"/>
+      <c r="B61" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E61" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A55:E55"/>
+  <mergeCells count="18">
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
-    <mergeCell ref="E56:E60"/>
+    <mergeCell ref="E56:E61"/>
     <mergeCell ref="E2:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="E14:E19"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="A28:E28"/>
@@ -2852,17 +3047,22 @@
     <mergeCell ref="E29:E33"/>
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="E35:E40"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png"/>
-    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png"/>
-    <hyperlink ref="E2:E12" r:id="rId3" display="TaskList1.png"/>
-    <hyperlink ref="E14:E19" r:id="rId4" display="QuickAdd.png"/>
-    <hyperlink ref="E29:E33" r:id="rId5" display="TasksDue.png"/>
-    <hyperlink ref="E35:E40" r:id="rId6" display="TasksStarting.png"/>
-    <hyperlink ref="E42:E47" r:id="rId7" display="TasksPriority.png"/>
-    <hyperlink ref="E49:E54" r:id="rId8" display="TaskProgress.png"/>
-    <hyperlink ref="E56:E60" r:id="rId9" display="Search.png"/>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{41B9DE7C-F513-7A4C-9608-80B8C1A2E0C8}"/>
+    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png" xr:uid="{FFDED12F-6E60-764B-AC50-E9A151FE766C}"/>
+    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png" xr:uid="{D4E49EAD-B8B9-0A49-B1A0-60F7A38DE2EA}"/>
+    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png" xr:uid="{ABDF668C-400D-2A4E-86EB-E9FD7C44BF55}"/>
+    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png" xr:uid="{DF68C727-EFA0-7542-B392-52D12BE8F88E}"/>
+    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png" xr:uid="{226D5616-AE1A-D140-B96F-B62F1F00654E}"/>
+    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png" xr:uid="{ED8A8934-31FF-2741-88B1-D7C03C047E87}"/>
+    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png" xr:uid="{152810F4-07BC-2D49-9C95-15E7C17419AF}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{8E6C32E5-2FBC-974B-A364-C1B820563A7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2870,24 +3070,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="116" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="78" style="11" customWidth="1"/>
+    <col min="2" max="2" width="97.83203125" style="11" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="29" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="22" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2898,56 +3098,56 @@
         <v>107</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="39" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="46" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="E3" s="47"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="40"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="47"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="22" t="s">
         <v>140</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
@@ -2955,58 +3155,60 @@
         <v>80</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="33"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" s="33"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="22" t="s">
         <v>144</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="33"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
         <v>146</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="33"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
         <v>148</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="33"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
         <v>78</v>
       </c>
@@ -3014,13 +3216,13 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
@@ -3028,11 +3230,11 @@
         <v>77</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E13" s="33"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
         <v>36</v>
       </c>
@@ -3040,518 +3242,573 @@
         <v>79</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E14" s="33"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E15" s="33"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E15" s="35"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="E16" s="33"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="33"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
         <v>112</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="33"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
         <v>113</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="33"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="35"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
         <v>83</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="33"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="33"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="35"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
         <v>115</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="33"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="35"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
         <v>116</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="33" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="33"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="44"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="33"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="E26" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="33"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="E27" s="44"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="33"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="E28" s="44"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B29" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="33"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="E29" s="33"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="E29" s="44"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="E30" s="44"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="41"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="E31" s="35" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="41"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E32" s="41"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="E33" s="35"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="41"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="35"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="35"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" s="35"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="35"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="11" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="E35" s="41"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="E36" s="41"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="E37" s="41"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="E38" s="41"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="B42" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="E42" s="33" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="E43" s="35"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="E44" s="35"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="E45" s="35"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="E46" s="35"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="E47" s="35"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="E48" s="35"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="39"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="E51" s="33" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="E41" s="32" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B42" s="15" t="s">
+      <c r="B52" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="E42" s="33"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="E43" s="33"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="15"/>
-      <c r="E44" s="33"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="E45" s="33"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="15"/>
-      <c r="E46" s="33"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="E47" s="33"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="31"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="15"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="15"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="C52" s="15"/>
+      <c r="E52" s="35"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B53" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="15"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="C53" s="15"/>
+      <c r="E53" s="35"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B54" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="15"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="C54" s="15"/>
+      <c r="E54" s="35"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B55" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="15"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+      <c r="C55" s="15"/>
+      <c r="E55" s="35"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B56" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="C56" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="E56" s="35"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="15" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="C57" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="E57" s="35"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="15"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="C58" s="15"/>
+      <c r="E58" s="35"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C58" s="15"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="C59" s="15"/>
+      <c r="E59" s="35"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B60" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>164</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>315</v>
+        <v>198</v>
+      </c>
+      <c r="E60" s="35" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="B61" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E61" s="35"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B62" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C61" s="15"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="C62" s="15"/>
+      <c r="E62" s="35"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B63" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="C62" s="15"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+      <c r="C63" s="15"/>
+      <c r="E63" s="35" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B64" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="C63" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="E64" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="E12:E22"/>
-    <mergeCell ref="E23:E29"/>
+  <mergeCells count="14">
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E26:E30"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="E42:E48"/>
+    <mergeCell ref="E51:E59"/>
+    <mergeCell ref="E60:E62"/>
     <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="E12:E22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png"/>
-    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png"/>
-    <hyperlink ref="E23:E29" r:id="rId5" display="EditTask2.png"/>
-    <hyperlink ref="E34" r:id="rId6"/>
-    <hyperlink ref="E39" r:id="rId7"/>
-    <hyperlink ref="E41:E47" r:id="rId8" display="Calendar.png"/>
-    <hyperlink ref="E48" r:id="rId9"/>
+    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{9FE2AE8E-A9CA-964E-A11C-56069919D277}"/>
+    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{AF945763-504F-F44B-941F-F68473F43173}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{C90C6E02-C85B-3048-B0C9-FEDCC070B8E1}"/>
+    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{7200B3E4-19A9-E34E-B217-AC9A8F0454BD}"/>
+    <hyperlink ref="E35" r:id="rId5" xr:uid="{8446D4E4-077D-0A4D-8525-8FB07FF0C373}"/>
+    <hyperlink ref="E40" r:id="rId6" xr:uid="{12FBB57A-780E-814C-87D8-AFBFE84831F1}"/>
+    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png" xr:uid="{610945C3-6CA0-044C-8FF8-83DD72D73D6A}"/>
+    <hyperlink ref="E49" r:id="rId8" xr:uid="{7E1BB3A1-2AEF-CA43-9C3D-463F6622F876}"/>
+    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png" xr:uid="{AAD316A3-DB94-4240-B398-3FB32A25F9D3}"/>
+    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png" xr:uid="{17A3A39B-02B6-714F-9B1B-FD402BDF5ABA}"/>
+    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png" xr:uid="{AB6376ED-61CD-AD4E-B9AC-DB5009AA4A5C}"/>
+    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png" xr:uid="{727B6477-B8DF-D142-8C44-57DAF56E23D5}"/>
+    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png" xr:uid="{FDC259CA-E4C3-6746-98E2-92665C5A49E4}"/>
+    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png" xr:uid="{D0EA7266-482F-8D4F-8F27-B9084ABDA77D}"/>
+    <hyperlink ref="E25" r:id="rId15" xr:uid="{ACC8DD5A-7237-0E49-90A1-C93B1602CF73}"/>
+    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png" xr:uid="{E529EFF7-B7A1-524E-A663-6A19E3F92017}"/>
+    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png" xr:uid="{1A63B7F9-20A8-9A47-844C-ED1A1163AB29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3559,23 +3816,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="28.83203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="118.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="123.5" style="11" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="31.1640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3586,215 +3845,272 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="33" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="35"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="21" t="s">
         <v>331</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="B9" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="20" t="s">
         <v>332</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="B10" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>334</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="20" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="B12" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
         <v>209</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="35"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>232</v>
-      </c>
       <c r="C16" s="11" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
         <v>212</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
         <v>215</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="50"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="33" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
+      <c r="E22" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A20:D20"/>
+  <mergeCells count="5">
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E10:E18"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png" xr:uid="{DBDAF80C-9383-FC40-B83E-398C0807592C}"/>
+    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png" xr:uid="{B769E664-C3A5-C846-8710-7122F377D25C}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{C5D88C3A-F299-6B4E-A9FD-59313F307545}"/>
+    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png" xr:uid="{4DF7ABBB-AA92-2E44-9C4D-E9A866C1708E}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{FFBC2EC3-5D16-8D4F-B3A3-FD8D1BDC8A1D}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{5752B374-7244-E240-924D-FA39114A1383}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
     <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
     <col min="4" max="4" width="14" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3805,240 +4121,294 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="33" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="E5" s="35"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="E6" s="35"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="11" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>287</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="35"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="11" t="s">
         <v>341</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>288</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="36"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="35"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="E21" s="35"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="E22" s="35"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="36"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="33" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>74</v>
       </c>
+      <c r="E26" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A24:D24"/>
+  <mergeCells count="9">
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A24:E24"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png" xr:uid="{1518F90C-C848-0E46-88B7-B89C8E1E7D4F}"/>
+    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png" xr:uid="{F7868AFA-E3A6-B44F-AABF-FEA46C17919B}"/>
+    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png" xr:uid="{C73A2777-D611-CD43-B9B4-C3594113B832}"/>
+    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png" xr:uid="{BC8B5071-BD9D-AA4A-8E01-D45B59CDDA17}"/>
+    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png" xr:uid="{BC664D47-EA3F-AC44-98C4-CB0A219B6118}"/>
+    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png" xr:uid="{BC31547B-6FE5-0843-A8E3-700C667AFBF5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9A35-BE5A-E64F-9080-864E7183DD30}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="107.6640625" style="11" customWidth="1"/>
@@ -4054,7 +4424,7 @@
     <col min="12" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -4065,7 +4435,7 @@
         <v>106</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -4089,7 +4459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -4106,7 +4476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -4123,7 +4493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -4140,7 +4510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -4159,7 +4529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -4178,7 +4548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -4197,7 +4567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -4216,7 +4586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -4232,7 +4602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -4250,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -4274,7 +4644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
@@ -4296,12 +4666,12 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4311,7 +4681,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="11" t="s">
         <v>57</v>
       </c>
@@ -4328,7 +4698,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="11" t="s">
         <v>56</v>
       </c>
@@ -4345,7 +4715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
@@ -4361,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="11" t="s">
         <v>49</v>
       </c>
@@ -4370,7 +4740,7 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>31</v>
@@ -4385,7 +4755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
@@ -4404,7 +4774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
@@ -4423,12 +4793,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+    <row r="20" spans="1:11">
+      <c r="A20" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -4438,7 +4808,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="11" t="s">
         <v>28</v>
       </c>
@@ -4452,7 +4822,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="11" t="s">
         <v>111</v>
       </c>
@@ -4460,7 +4830,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="11" t="s">
         <v>30</v>
       </c>
@@ -4474,7 +4844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
@@ -4488,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="11" t="s">
         <v>32</v>
       </c>
@@ -4496,7 +4866,7 @@
         <v>80</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>8</v>
@@ -4508,7 +4878,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="11" t="s">
         <v>34</v>
       </c>
@@ -4525,7 +4895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="11" t="s">
         <v>142</v>
       </c>
@@ -4533,7 +4903,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="11" t="s">
         <v>144</v>
       </c>
@@ -4550,7 +4920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="11" t="s">
         <v>146</v>
       </c>
@@ -4567,7 +4937,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="11" t="s">
         <v>148</v>
       </c>
@@ -4590,7 +4960,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="11" t="s">
         <v>78</v>
       </c>
@@ -4613,7 +4983,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="11" t="s">
         <v>35</v>
       </c>
@@ -4621,10 +4991,10 @@
         <v>77</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="11" t="s">
         <v>36</v>
       </c>
@@ -4632,10 +5002,10 @@
         <v>79</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="11" t="s">
         <v>39</v>
       </c>
@@ -4646,10 +5016,10 @@
         <v>139</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
@@ -4660,7 +5030,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="11" t="s">
         <v>82</v>
       </c>
@@ -4668,7 +5038,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="11" t="s">
         <v>112</v>
       </c>
@@ -4676,7 +5046,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="11" t="s">
         <v>113</v>
       </c>
@@ -4684,7 +5054,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="11" t="s">
         <v>83</v>
       </c>
@@ -4692,7 +5062,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="11" t="s">
         <v>114</v>
       </c>
@@ -4700,7 +5070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="11" t="s">
         <v>115</v>
       </c>
@@ -4708,7 +5078,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="11" t="s">
         <v>116</v>
       </c>
@@ -4716,7 +5086,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="11" t="s">
         <v>117</v>
       </c>
@@ -4724,7 +5094,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="11" t="s">
         <v>118</v>
       </c>
@@ -4732,7 +5102,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="11" t="s">
         <v>119</v>
       </c>
@@ -4740,7 +5110,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="11" t="s">
         <v>120</v>
       </c>
@@ -4748,7 +5118,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="11" t="s">
         <v>172</v>
       </c>
@@ -4759,7 +5129,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="11" t="s">
         <v>171</v>
       </c>
@@ -4767,7 +5137,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="11" t="s">
         <v>180</v>
       </c>
@@ -4775,7 +5145,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="11" t="s">
         <v>181</v>
       </c>
@@ -4783,7 +5153,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="11" t="s">
         <v>182</v>
       </c>
@@ -4791,7 +5161,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="11" t="s">
         <v>183</v>
       </c>
@@ -4799,7 +5169,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="11" t="s">
         <v>173</v>
       </c>
@@ -4807,7 +5177,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="11" t="s">
         <v>188</v>
       </c>
@@ -4815,7 +5185,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="11" t="s">
         <v>189</v>
       </c>
@@ -4823,7 +5193,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="11" t="s">
         <v>190</v>
       </c>
@@ -4831,7 +5201,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="11" t="s">
         <v>191</v>
       </c>
@@ -4839,7 +5209,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="11" t="s">
         <v>174</v>
       </c>
@@ -4847,18 +5217,18 @@
         <v>178</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="31"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="39"/>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
         <v>121</v>
       </c>
@@ -4866,7 +5236,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="11" t="s">
         <v>122</v>
       </c>
@@ -4874,7 +5244,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="11" t="s">
         <v>123</v>
       </c>
@@ -4882,7 +5252,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="11" t="s">
         <v>124</v>
       </c>
@@ -4892,7 +5262,7 @@
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="11" t="s">
         <v>125</v>
       </c>
@@ -4902,7 +5272,7 @@
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="11" t="s">
         <v>126</v>
       </c>
@@ -4912,7 +5282,7 @@
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="11" t="s">
         <v>127</v>
       </c>
@@ -4924,7 +5294,7 @@
       </c>
       <c r="D66" s="15"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="11" t="s">
         <v>128</v>
       </c>
@@ -4936,15 +5306,15 @@
       </c>
       <c r="D67" s="15"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="29" t="s">
+    <row r="68" spans="1:4">
+      <c r="A68" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="31"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="39"/>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
         <v>129</v>
       </c>
@@ -4954,7 +5324,7 @@
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="11" t="s">
         <v>130</v>
       </c>
@@ -4964,7 +5334,7 @@
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="11" t="s">
         <v>131</v>
       </c>
@@ -4974,7 +5344,7 @@
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="11" t="s">
         <v>132</v>
       </c>
@@ -4984,7 +5354,7 @@
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="11" t="s">
         <v>133</v>
       </c>
@@ -4994,7 +5364,7 @@
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="11" t="s">
         <v>134</v>
       </c>
@@ -5006,7 +5376,7 @@
       </c>
       <c r="D74" s="15"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="11" t="s">
         <v>135</v>
       </c>
@@ -5018,7 +5388,7 @@
       </c>
       <c r="D75" s="15"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="11" t="s">
         <v>136</v>
       </c>
@@ -5028,7 +5398,7 @@
       <c r="C76" s="15"/>
       <c r="D76" s="15"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="11" t="s">
         <v>137</v>
       </c>
@@ -5038,7 +5408,7 @@
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="11" t="s">
         <v>162</v>
       </c>
@@ -5047,10 +5417,10 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="11" t="s">
         <v>161</v>
       </c>
@@ -5059,10 +5429,10 @@
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="11" t="s">
         <v>165</v>
       </c>
@@ -5072,7 +5442,7 @@
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="11" t="s">
         <v>167</v>
       </c>
@@ -5082,7 +5452,7 @@
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="11" t="s">
         <v>168</v>
       </c>
@@ -5092,11 +5462,11 @@
       <c r="C82" s="15"/>
       <c r="D82" s="15"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="29"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="31"/>
+    <row r="83" spans="1:4">
+      <c r="A83" s="37"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Add RestartCommand, RestartAndCleanCommand and PressPercentageCommand.
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1466C0-70D8-FD45-B070-607A89299BD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00885372-A7DF-BE47-827B-20667072F503}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="5760" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ViewTask!$A$1:$A$10</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="393">
   <si>
     <t>component</t>
   </si>
@@ -1766,6 +1766,9 @@
   </si>
   <si>
     <t>PickColor.png</t>
+  </si>
+  <si>
+    <t>//*[@index='10']//android.widget.SeekBar</t>
   </si>
 </sst>
 </file>
@@ -2007,14 +2010,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2025,7 +2026,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2050,22 +2069,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2385,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56:E61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2423,7 +2426,7 @@
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="39" t="s">
         <v>371</v>
       </c>
     </row>
@@ -2434,7 +2437,7 @@
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
@@ -2443,7 +2446,7 @@
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
@@ -2453,7 +2456,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="31"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
@@ -2463,7 +2466,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="31"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
@@ -2473,7 +2476,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="31"/>
+      <c r="E7" s="40"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
@@ -2483,7 +2486,7 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="31"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
@@ -2493,7 +2496,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="31"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
@@ -2505,7 +2508,7 @@
       <c r="C10" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
@@ -2517,7 +2520,7 @@
       <c r="C11" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
@@ -2529,7 +2532,7 @@
       <c r="C12" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="41"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="33" t="s">
@@ -2547,7 +2550,7 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="36" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2558,7 +2561,7 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
@@ -2573,7 +2576,7 @@
       <c r="E16" s="27" t="s">
         <v>372</v>
       </c>
-      <c r="F16" s="49"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -2585,7 +2588,7 @@
       <c r="D17" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="37" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2596,7 +2599,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="37"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2605,7 +2608,7 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="48"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="33" t="s">
@@ -2623,7 +2626,7 @@
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="39" t="s">
         <v>290</v>
       </c>
     </row>
@@ -2634,7 +2637,7 @@
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="32"/>
+      <c r="E22" s="41"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="33" t="s">
@@ -2652,7 +2655,7 @@
       <c r="B24" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="39" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2663,7 +2666,7 @@
       <c r="B25" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E25" s="31"/>
+      <c r="E25" s="40"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
@@ -2672,7 +2675,7 @@
       <c r="B26" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="31"/>
+      <c r="E26" s="40"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
@@ -2681,7 +2684,7 @@
       <c r="B27" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E27" s="32"/>
+      <c r="E27" s="41"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="33" t="s">
@@ -2699,7 +2702,7 @@
       <c r="B29" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="39" t="s">
         <v>292</v>
       </c>
     </row>
@@ -2710,7 +2713,7 @@
       <c r="B30" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="31"/>
+      <c r="E30" s="40"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
@@ -2719,7 +2722,7 @@
       <c r="B31" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E31" s="31"/>
+      <c r="E31" s="40"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
@@ -2728,7 +2731,7 @@
       <c r="B32" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E32" s="31"/>
+      <c r="E32" s="40"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
@@ -2740,7 +2743,7 @@
       <c r="C33" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E33" s="32"/>
+      <c r="E33" s="41"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="33" t="s">
@@ -2759,7 +2762,7 @@
         <v>258</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="39" t="s">
         <v>293</v>
       </c>
     </row>
@@ -2770,7 +2773,7 @@
       <c r="B36" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="40"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
@@ -2779,7 +2782,7 @@
       <c r="B37" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E37" s="31"/>
+      <c r="E37" s="40"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="13" t="s">
@@ -2788,7 +2791,7 @@
       <c r="B38" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="40"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
@@ -2797,7 +2800,7 @@
       <c r="B39" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E39" s="31"/>
+      <c r="E39" s="40"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
@@ -2809,16 +2812,16 @@
       <c r="C40" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E40" s="32"/>
+      <c r="E40" s="41"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="43" t="s">
         <v>276</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="45"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
@@ -2828,7 +2831,7 @@
         <v>260</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="39" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2839,7 +2842,7 @@
       <c r="B43" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="E43" s="31"/>
+      <c r="E43" s="40"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -2848,7 +2851,7 @@
       <c r="B44" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="E44" s="31"/>
+      <c r="E44" s="40"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -2857,7 +2860,7 @@
       <c r="B45" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="E45" s="31"/>
+      <c r="E45" s="40"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -2869,7 +2872,7 @@
       <c r="C46" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E46" s="31"/>
+      <c r="E46" s="40"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -2881,7 +2884,7 @@
       <c r="C47" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E47" s="32"/>
+      <c r="E47" s="41"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="33" t="s">
@@ -2900,7 +2903,7 @@
         <v>261</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="E49" s="30" t="s">
+      <c r="E49" s="39" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2911,7 +2914,7 @@
       <c r="B50" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="E50" s="31"/>
+      <c r="E50" s="40"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -2920,7 +2923,7 @@
       <c r="B51" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="E51" s="31"/>
+      <c r="E51" s="40"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
@@ -2929,7 +2932,7 @@
       <c r="B52" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="E52" s="31"/>
+      <c r="E52" s="40"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -2938,7 +2941,7 @@
       <c r="B53" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E53" s="31"/>
+      <c r="E53" s="40"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -2950,7 +2953,7 @@
       <c r="C54" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E54" s="32"/>
+      <c r="E54" s="41"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="33" t="s">
@@ -2972,7 +2975,7 @@
       <c r="D56" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E56" s="30" t="s">
+      <c r="E56" s="39" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2984,7 +2987,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="E57" s="45"/>
+      <c r="E57" s="42"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -2993,7 +2996,7 @@
       <c r="B58" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="E58" s="31"/>
+      <c r="E58" s="40"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3005,7 +3008,7 @@
       <c r="C59" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E59" s="31"/>
+      <c r="E59" s="40"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="14" t="s">
@@ -3017,7 +3020,7 @@
       <c r="C60" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E60" s="31"/>
+      <c r="E60" s="40"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="11" t="s">
@@ -3029,15 +3032,10 @@
       <c r="C61" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E61" s="31"/>
+      <c r="E61" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
     <mergeCell ref="E2:E12"/>
     <mergeCell ref="A13:E13"/>
@@ -3051,6 +3049,11 @@
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="E49:E54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
@@ -3073,8 +3076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3111,7 +3114,7 @@
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="46" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3122,7 +3125,7 @@
       <c r="B3" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="E3" s="41"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
@@ -3131,7 +3134,7 @@
       <c r="B4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="47"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="22" t="s">
@@ -3157,7 +3160,7 @@
       <c r="D6" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="40" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3168,7 +3171,7 @@
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="40"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
@@ -3177,7 +3180,7 @@
       <c r="B8" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="40" t="s">
         <v>376</v>
       </c>
     </row>
@@ -3188,7 +3191,7 @@
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
@@ -3197,7 +3200,7 @@
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
@@ -3206,7 +3209,7 @@
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -3218,7 +3221,7 @@
       <c r="C12" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="40" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3232,7 +3235,7 @@
       <c r="D13" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3244,7 +3247,7 @@
       <c r="D14" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -3259,7 +3262,7 @@
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
@@ -3271,7 +3274,7 @@
       <c r="C16" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -3280,7 +3283,7 @@
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="31"/>
+      <c r="E17" s="40"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -3289,7 +3292,7 @@
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="31"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -3298,7 +3301,7 @@
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="31"/>
+      <c r="E19" s="40"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -3307,7 +3310,7 @@
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="40"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -3316,7 +3319,7 @@
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="40"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -3325,7 +3328,7 @@
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="40"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -3334,7 +3337,7 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="37" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3345,7 +3348,7 @@
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="37"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
@@ -3360,7 +3363,7 @@
       <c r="D25" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="E25" s="50" t="s">
+      <c r="E25" s="32" t="s">
         <v>379</v>
       </c>
     </row>
@@ -3371,7 +3374,7 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="37" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3382,7 +3385,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="37"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3391,16 +3394,16 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="36"/>
+      <c r="E28" s="37"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
         <v>172</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" s="36"/>
+        <v>392</v>
+      </c>
+      <c r="E29" s="37"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
@@ -3409,7 +3412,7 @@
       <c r="B30" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="37"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3418,7 +3421,7 @@
       <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="40" t="s">
         <v>377</v>
       </c>
     </row>
@@ -3429,7 +3432,7 @@
       <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="31"/>
+      <c r="E32" s="40"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3438,7 +3441,7 @@
       <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E33" s="31"/>
+      <c r="E33" s="40"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
@@ -3447,7 +3450,7 @@
       <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="31"/>
+      <c r="E34" s="40"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
@@ -3467,7 +3470,7 @@
       <c r="B36" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="40" t="s">
         <v>378</v>
       </c>
     </row>
@@ -3478,7 +3481,7 @@
       <c r="B37" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="31"/>
+      <c r="E37" s="40"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3487,7 +3490,7 @@
       <c r="B38" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="40"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="22" t="s">
@@ -3496,7 +3499,7 @@
       <c r="B39" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="31"/>
+      <c r="E39" s="40"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
@@ -3529,7 +3532,7 @@
         <v>73</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="39" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3541,7 +3544,7 @@
         <v>74</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="31"/>
+      <c r="E43" s="40"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -3551,7 +3554,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="31"/>
+      <c r="E44" s="40"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -3561,7 +3564,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="31"/>
+      <c r="E45" s="40"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -3571,7 +3574,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="31"/>
+      <c r="E46" s="40"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -3581,7 +3584,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="E47" s="31"/>
+      <c r="E47" s="40"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
@@ -3593,7 +3596,7 @@
       <c r="C48" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="E48" s="31"/>
+      <c r="E48" s="40"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="11" t="s">
@@ -3626,7 +3629,7 @@
         <v>73</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="E51" s="30" t="s">
+      <c r="E51" s="39" t="s">
         <v>373</v>
       </c>
     </row>
@@ -3638,7 +3641,7 @@
         <v>74</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="E52" s="31"/>
+      <c r="E52" s="40"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -3648,7 +3651,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="E53" s="31"/>
+      <c r="E53" s="40"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -3658,7 +3661,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="E54" s="31"/>
+      <c r="E54" s="40"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
@@ -3668,7 +3671,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="E55" s="31"/>
+      <c r="E55" s="40"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="11" t="s">
@@ -3680,7 +3683,7 @@
       <c r="C56" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="E56" s="31"/>
+      <c r="E56" s="40"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
@@ -3692,7 +3695,7 @@
       <c r="C57" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="E57" s="31"/>
+      <c r="E57" s="40"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3702,7 +3705,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="E58" s="31"/>
+      <c r="E58" s="40"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3712,7 +3715,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="E59" s="31"/>
+      <c r="E59" s="40"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="13" t="s">
@@ -3725,7 +3728,7 @@
       <c r="D60" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E60" s="31" t="s">
+      <c r="E60" s="40" t="s">
         <v>374</v>
       </c>
     </row>
@@ -3740,7 +3743,7 @@
       <c r="D61" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E61" s="31"/>
+      <c r="E61" s="40"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
@@ -3750,7 +3753,7 @@
         <v>166</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="E62" s="31"/>
+      <c r="E62" s="40"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="22" t="s">
@@ -3760,7 +3763,7 @@
         <v>169</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="E63" s="31" t="s">
+      <c r="E63" s="40" t="s">
         <v>375</v>
       </c>
     </row>
@@ -3772,7 +3775,7 @@
         <v>170</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="E64" s="31"/>
+      <c r="E64" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3858,7 +3861,7 @@
       <c r="B2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="39" t="s">
         <v>380</v>
       </c>
     </row>
@@ -3869,7 +3872,7 @@
       <c r="B3" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
@@ -3878,7 +3881,7 @@
       <c r="B4" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
@@ -3887,7 +3890,7 @@
       <c r="B5" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
@@ -3896,7 +3899,7 @@
       <c r="B6" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="40" t="s">
         <v>383</v>
       </c>
     </row>
@@ -3907,7 +3910,7 @@
       <c r="B7" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="40"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
@@ -3938,7 +3941,7 @@
       <c r="B10" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="40" t="s">
         <v>380</v>
       </c>
     </row>
@@ -3949,7 +3952,7 @@
       <c r="B11" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
@@ -3958,7 +3961,7 @@
       <c r="B12" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="40"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
@@ -3967,7 +3970,7 @@
       <c r="B13" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3979,7 +3982,7 @@
       <c r="C14" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -3994,10 +3997,10 @@
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="30" t="s">
         <v>211</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -4006,7 +4009,7 @@
       <c r="C16" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
@@ -4015,7 +4018,7 @@
       <c r="B17" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E17" s="31"/>
+      <c r="E17" s="40"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
@@ -4024,7 +4027,7 @@
       <c r="B18" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="31"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
@@ -4044,13 +4047,13 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="48" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="44"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="50"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -4059,7 +4062,7 @@
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="39" t="s">
         <v>382</v>
       </c>
     </row>
@@ -4070,7 +4073,7 @@
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4134,7 +4137,7 @@
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="39" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4145,7 +4148,7 @@
       <c r="B3" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
@@ -4157,7 +4160,7 @@
       <c r="C4" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
@@ -4169,7 +4172,7 @@
       <c r="C5" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
@@ -4178,7 +4181,7 @@
       <c r="B6" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
@@ -4187,7 +4190,7 @@
       <c r="B7" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="40" t="s">
         <v>390</v>
       </c>
     </row>
@@ -4198,7 +4201,7 @@
       <c r="B8" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="41"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="33" t="s">
@@ -4219,7 +4222,7 @@
       <c r="D10" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="39" t="s">
         <v>388</v>
       </c>
     </row>
@@ -4230,7 +4233,7 @@
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -4239,7 +4242,7 @@
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="40"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
@@ -4248,7 +4251,7 @@
       <c r="B13" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="40" t="s">
         <v>386</v>
       </c>
     </row>
@@ -4259,7 +4262,7 @@
       <c r="B14" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -4268,7 +4271,7 @@
       <c r="B15" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
@@ -4277,7 +4280,7 @@
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="32"/>
+      <c r="E16" s="41"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="33" t="s">
@@ -4298,7 +4301,7 @@
       <c r="C18" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="39" t="s">
         <v>391</v>
       </c>
     </row>
@@ -4309,7 +4312,7 @@
       <c r="B19" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E19" s="31"/>
+      <c r="E19" s="40"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -4318,7 +4321,7 @@
       <c r="B20" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="40"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -4327,7 +4330,7 @@
       <c r="B21" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="40"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -4336,7 +4339,7 @@
       <c r="B22" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="40"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -4345,16 +4348,16 @@
       <c r="B23" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="E23" s="32"/>
+      <c r="E23" s="41"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="48" t="s">
         <v>284</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
@@ -4363,7 +4366,7 @@
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="39" t="s">
         <v>389</v>
       </c>
     </row>
@@ -4374,7 +4377,7 @@
       <c r="B26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="31"/>
+      <c r="E26" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4794,11 +4797,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>

</xml_diff>

<commit_message>
Add search function test script
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF685BD2-B1C8-6E40-A6F8-00E2312A4B1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCD5A3C-5A96-9544-889F-061BB7D76847}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="1160" yWindow="1100" windowWidth="29260" windowHeight="17420" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -864,28 +864,6 @@
     <t>//*[@text='not specified']</t>
   </si>
   <si>
-    <r>
-      <t>//*[@text='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${NAME}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']</t>
-    </r>
-  </si>
-  <si>
     <t>Input field</t>
   </si>
   <si>
@@ -1772,6 +1750,28 @@
   </si>
   <si>
     <t>//*[@index='0']//*[@class='android.widget.EditText']</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.TextView' and @text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}']</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2023,13 +2023,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2391,8 +2391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2416,10 +2416,10 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2430,7 +2430,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2440,7 +2440,7 @@
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
@@ -2449,7 +2449,7 @@
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
@@ -2459,7 +2459,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
@@ -2469,7 +2469,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="35"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
@@ -2479,7 +2479,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
@@ -2489,29 +2489,29 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="35"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="35"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E10" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
@@ -2521,25 +2521,25 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="E11" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E12" s="36"/>
+        <v>341</v>
+      </c>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
@@ -2554,7 +2554,7 @@
         <v>70</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2571,13 +2571,13 @@
         <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F16" s="31"/>
     </row>
@@ -2589,10 +2589,10 @@
         <v>72</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2615,7 +2615,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -2624,27 +2624,27 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -2653,45 +2653,45 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="E25" s="35"/>
+        <v>222</v>
+      </c>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" s="35"/>
+        <v>223</v>
+      </c>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="E27" s="36"/>
+        <v>224</v>
+      </c>
+      <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="37" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
@@ -2700,57 +2700,57 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E30" s="35"/>
+        <v>254</v>
+      </c>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E31" s="35"/>
+        <v>255</v>
+      </c>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E32" s="35"/>
+        <v>256</v>
+      </c>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E33" s="36"/>
+        <v>341</v>
+      </c>
+      <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="37" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -2759,67 +2759,67 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C35" s="7"/>
       <c r="E35" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E36" s="35"/>
+        <v>253</v>
+      </c>
+      <c r="E36" s="34"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E37" s="35"/>
+        <v>254</v>
+      </c>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E38" s="35"/>
+        <v>256</v>
+      </c>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="E39" s="35"/>
+        <v>258</v>
+      </c>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E40" s="36"/>
+        <v>341</v>
+      </c>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B41" s="41"/>
       <c r="C41" s="41"/>
@@ -2828,42 +2828,42 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C42" s="7"/>
       <c r="E42" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="E43" s="35"/>
+        <v>359</v>
+      </c>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="E44" s="35"/>
+        <v>360</v>
+      </c>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="E45" s="35"/>
+        <v>361</v>
+      </c>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -2873,25 +2873,25 @@
         <v>138</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="E46" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E47" s="36"/>
+        <v>341</v>
+      </c>
+      <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B48" s="38"/>
       <c r="C48" s="38"/>
@@ -2900,67 +2900,67 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C49" s="7"/>
       <c r="E49" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="E50" s="35"/>
+        <v>261</v>
+      </c>
+      <c r="E50" s="34"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="E51" s="35"/>
+        <v>262</v>
+      </c>
+      <c r="E51" s="34"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="E52" s="35"/>
+        <v>263</v>
+      </c>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E53" s="35"/>
+        <v>264</v>
+      </c>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E54" s="36"/>
+        <v>341</v>
+      </c>
+      <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B55" s="38"/>
       <c r="C55" s="38"/>
@@ -2969,76 +2969,78 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="E57" s="34"/>
+      <c r="E57" s="36"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="E58" s="35"/>
+        <v>267</v>
+      </c>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="E59" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="14" t="s">
         <v>141</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E60" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E60" s="34"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>196</v>
+        <v>393</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E61" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E61" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
@@ -3055,8 +3057,6 @@
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A55:E55"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
@@ -3079,8 +3079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A10" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3104,10 +3104,10 @@
         <v>107</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3118,21 +3118,21 @@
         <v>76</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>71</v>
@@ -3144,13 +3144,13 @@
         <v>140</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3158,33 +3158,33 @@
         <v>32</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>302</v>
+        <v>198</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>376</v>
+        <v>352</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3194,7 +3194,7 @@
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
@@ -3203,7 +3203,7 @@
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
@@ -3212,7 +3212,7 @@
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -3222,10 +3222,10 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>302</v>
+        <v>342</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3236,9 +3236,9 @@
         <v>77</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E13" s="35"/>
+        <v>198</v>
+      </c>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3248,36 +3248,36 @@
         <v>79</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E14" s="35"/>
+        <v>198</v>
+      </c>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="35"/>
+        <v>198</v>
+      </c>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E16" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -3286,7 +3286,7 @@
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -3295,7 +3295,7 @@
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -3304,7 +3304,7 @@
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -3313,7 +3313,7 @@
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -3322,7 +3322,7 @@
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -3331,7 +3331,7 @@
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -3341,12 +3341,12 @@
         <v>84</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>85</v>
@@ -3355,19 +3355,19 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>357</v>
-      </c>
       <c r="C25" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3378,7 +3378,7 @@
         <v>92</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3404,16 +3404,16 @@
         <v>172</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E29" s="44"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E30" s="44"/>
     </row>
@@ -3424,8 +3424,8 @@
       <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="35" t="s">
-        <v>377</v>
+      <c r="E31" s="34" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3435,7 +3435,7 @@
       <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="35"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3444,7 +3444,7 @@
       <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E33" s="35"/>
+      <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
@@ -3453,17 +3453,17 @@
       <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="35"/>
+      <c r="E34" s="34"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3473,8 +3473,8 @@
       <c r="B36" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="35" t="s">
-        <v>378</v>
+      <c r="E36" s="34" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3484,7 +3484,7 @@
       <c r="B37" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="35"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3493,7 +3493,7 @@
       <c r="B38" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="22" t="s">
@@ -3502,25 +3502,25 @@
       <c r="B39" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="35"/>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B41" s="38"/>
       <c r="C41" s="38"/>
@@ -3529,25 +3529,25 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="15"/>
       <c r="E42" s="33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="35"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -3557,7 +3557,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="35"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -3567,7 +3567,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="35"/>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -3577,7 +3577,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="35"/>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -3587,7 +3587,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="E47" s="35"/>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
@@ -3597,9 +3597,9 @@
         <v>154</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="E48" s="35"/>
+        <v>345</v>
+      </c>
+      <c r="E48" s="34"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="11" t="s">
@@ -3609,15 +3609,15 @@
         <v>153</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B50" s="38"/>
       <c r="C50" s="38"/>
@@ -3626,25 +3626,25 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C51" s="15"/>
       <c r="E51" s="33" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="E52" s="35"/>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -3654,7 +3654,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="E53" s="35"/>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -3664,7 +3664,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="E54" s="35"/>
+      <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
@@ -3674,7 +3674,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="E55" s="35"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="11" t="s">
@@ -3684,9 +3684,9 @@
         <v>157</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="E56" s="35"/>
+        <v>343</v>
+      </c>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
@@ -3696,9 +3696,9 @@
         <v>158</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="E57" s="35"/>
+        <v>344</v>
+      </c>
+      <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3708,7 +3708,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="E58" s="35"/>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3718,7 +3718,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="E59" s="35"/>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="13" t="s">
@@ -3729,10 +3729,10 @@
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E60" s="35" t="s">
-        <v>374</v>
+        <v>197</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3744,19 +3744,19 @@
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E61" s="35"/>
+        <v>197</v>
+      </c>
+      <c r="E61" s="34"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>166</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="E62" s="35"/>
+      <c r="E62" s="34"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="22" t="s">
@@ -3766,8 +3766,8 @@
         <v>169</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="E63" s="35" t="s">
-        <v>375</v>
+      <c r="E63" s="34" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3778,7 +3778,7 @@
         <v>170</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="E64" s="35"/>
+      <c r="E64" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3825,8 +3825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3851,207 +3851,207 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>67</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="35"/>
+        <v>209</v>
+      </c>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>383</v>
+        <v>216</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="E7" s="35"/>
+        <v>217</v>
+      </c>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>380</v>
+        <v>206</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="E11" s="35"/>
+        <v>207</v>
+      </c>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12" s="35"/>
+        <v>204</v>
+      </c>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="E13" s="35"/>
+        <v>364</v>
+      </c>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E14" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="35"/>
+        <v>198</v>
+      </c>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E16" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E18" s="35"/>
+        <v>213</v>
+      </c>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>368</v>
-      </c>
       <c r="E19" s="26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
@@ -4060,23 +4060,23 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4128,88 +4128,88 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E4" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E5" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="E6" s="35"/>
+        <v>232</v>
+      </c>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>390</v>
+        <v>251</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" s="36"/>
+        <v>252</v>
+      </c>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
@@ -4218,77 +4218,77 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>386</v>
+        <v>235</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="E14" s="35"/>
+        <v>236</v>
+      </c>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="E15" s="35"/>
+        <v>237</v>
+      </c>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -4297,66 +4297,66 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>249</v>
-      </c>
       <c r="C18" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E19" s="35"/>
+        <v>209</v>
+      </c>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="E20" s="35"/>
+        <v>238</v>
+      </c>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="E21" s="35"/>
+        <v>239</v>
+      </c>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="E22" s="35"/>
+        <v>240</v>
+      </c>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="E23" s="36"/>
+        <v>241</v>
+      </c>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -4365,23 +4365,23 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4442,7 +4442,7 @@
         <v>106</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>31</v>
@@ -4873,7 +4873,7 @@
         <v>80</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>8</v>
@@ -4998,7 +4998,7 @@
         <v>77</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5009,7 +5009,7 @@
         <v>79</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5023,7 +5023,7 @@
         <v>139</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5224,7 +5224,7 @@
         <v>178</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -5424,7 +5424,7 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -5436,7 +5436,7 @@
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:4">

</xml_diff>

<commit_message>
update scripts and test data
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF685BD2-B1C8-6E40-A6F8-00E2312A4B1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C7056-E542-B94F-A339-F36621D2B4EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="395">
   <si>
     <t>component</t>
   </si>
@@ -1772,6 +1772,9 @@
   </si>
   <si>
     <t>//*[@index='0']//*[@class='android.widget.EditText']</t>
+  </si>
+  <si>
+    <t>//*[@index='0' and @class='android.widget.ImageButton']</t>
   </si>
 </sst>
 </file>
@@ -2023,13 +2026,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2391,7 +2394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2440,7 +2443,7 @@
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
@@ -2449,7 +2452,7 @@
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
@@ -2459,7 +2462,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
@@ -2469,7 +2472,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="35"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
@@ -2479,7 +2482,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
@@ -2489,7 +2492,7 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="35"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
@@ -2499,7 +2502,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="35"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
@@ -2511,7 +2514,7 @@
       <c r="C10" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
@@ -2523,7 +2526,7 @@
       <c r="C11" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
@@ -2535,7 +2538,7 @@
       <c r="C12" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E12" s="36"/>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="37" t="s">
@@ -2640,7 +2643,7 @@
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="37" t="s">
@@ -2669,7 +2672,7 @@
       <c r="B25" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E25" s="35"/>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
@@ -2678,7 +2681,7 @@
       <c r="B26" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
@@ -2687,7 +2690,7 @@
       <c r="B27" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="37" t="s">
@@ -2716,7 +2719,7 @@
       <c r="B30" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="35"/>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
@@ -2725,7 +2728,7 @@
       <c r="B31" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E31" s="35"/>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
@@ -2734,7 +2737,7 @@
       <c r="B32" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E32" s="35"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
@@ -2746,7 +2749,7 @@
       <c r="C33" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E33" s="36"/>
+      <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="37" t="s">
@@ -2776,7 +2779,7 @@
       <c r="B36" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E36" s="35"/>
+      <c r="E36" s="34"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
@@ -2785,7 +2788,7 @@
       <c r="B37" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E37" s="35"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="13" t="s">
@@ -2794,7 +2797,7 @@
       <c r="B38" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
@@ -2803,7 +2806,7 @@
       <c r="B39" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E39" s="35"/>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
@@ -2815,7 +2818,7 @@
       <c r="C40" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E40" s="36"/>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="40" t="s">
@@ -2845,7 +2848,7 @@
       <c r="B43" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="E43" s="35"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -2854,7 +2857,7 @@
       <c r="B44" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="E44" s="35"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -2863,7 +2866,7 @@
       <c r="B45" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="E45" s="35"/>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -2875,7 +2878,7 @@
       <c r="C46" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E46" s="35"/>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -2887,7 +2890,7 @@
       <c r="C47" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E47" s="36"/>
+      <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="37" t="s">
@@ -2917,7 +2920,7 @@
       <c r="B50" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="E50" s="35"/>
+      <c r="E50" s="34"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -2926,7 +2929,7 @@
       <c r="B51" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="E51" s="35"/>
+      <c r="E51" s="34"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
@@ -2935,7 +2938,7 @@
       <c r="B52" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="E52" s="35"/>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -2944,7 +2947,7 @@
       <c r="B53" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E53" s="35"/>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -2956,7 +2959,7 @@
       <c r="C54" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E54" s="36"/>
+      <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="37" t="s">
@@ -2990,7 +2993,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="E57" s="34"/>
+      <c r="E57" s="36"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -2999,7 +3002,7 @@
       <c r="B58" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="E58" s="35"/>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3011,7 +3014,7 @@
       <c r="C59" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E59" s="35"/>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="14" t="s">
@@ -3023,7 +3026,7 @@
       <c r="C60" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E60" s="35"/>
+      <c r="E60" s="34"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="11" t="s">
@@ -3035,10 +3038,12 @@
       <c r="C61" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E61" s="35"/>
+      <c r="E61" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
@@ -3055,8 +3060,6 @@
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A55:E55"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
@@ -3080,7 +3083,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3163,7 +3166,7 @@
       <c r="D6" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3174,7 +3177,7 @@
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
@@ -3183,7 +3186,7 @@
       <c r="B8" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="34" t="s">
         <v>376</v>
       </c>
     </row>
@@ -3194,7 +3197,7 @@
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
@@ -3203,7 +3206,7 @@
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
@@ -3212,7 +3215,7 @@
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -3224,7 +3227,7 @@
       <c r="C12" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="34" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3238,7 +3241,7 @@
       <c r="D13" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3250,7 +3253,7 @@
       <c r="D14" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -3265,7 +3268,7 @@
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
@@ -3277,7 +3280,7 @@
       <c r="C16" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="35"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -3286,7 +3289,7 @@
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -3295,7 +3298,7 @@
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -3304,7 +3307,7 @@
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -3313,7 +3316,7 @@
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -3322,7 +3325,7 @@
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -3331,7 +3334,7 @@
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -3424,7 +3427,7 @@
       <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="34" t="s">
         <v>377</v>
       </c>
     </row>
@@ -3435,7 +3438,7 @@
       <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="35"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3444,7 +3447,7 @@
       <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E33" s="35"/>
+      <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
@@ -3453,7 +3456,7 @@
       <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="35"/>
+      <c r="E34" s="34"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
@@ -3473,7 +3476,7 @@
       <c r="B36" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E36" s="34" t="s">
         <v>378</v>
       </c>
     </row>
@@ -3484,7 +3487,7 @@
       <c r="B37" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="35"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3493,7 +3496,7 @@
       <c r="B38" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="22" t="s">
@@ -3502,7 +3505,7 @@
       <c r="B39" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="35"/>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
@@ -3547,7 +3550,7 @@
         <v>74</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="35"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -3557,7 +3560,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="35"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -3567,7 +3570,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="35"/>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -3577,7 +3580,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="35"/>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -3587,7 +3590,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="E47" s="35"/>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
@@ -3599,7 +3602,7 @@
       <c r="C48" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="E48" s="35"/>
+      <c r="E48" s="34"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="11" t="s">
@@ -3644,7 +3647,7 @@
         <v>74</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="E52" s="35"/>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -3654,7 +3657,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="E53" s="35"/>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -3664,7 +3667,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="E54" s="35"/>
+      <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
@@ -3674,7 +3677,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="E55" s="35"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="11" t="s">
@@ -3686,7 +3689,7 @@
       <c r="C56" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="E56" s="35"/>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
@@ -3698,7 +3701,7 @@
       <c r="C57" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="E57" s="35"/>
+      <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3708,7 +3711,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="E58" s="35"/>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3718,7 +3721,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="E59" s="35"/>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="13" t="s">
@@ -3731,7 +3734,7 @@
       <c r="D60" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E60" s="35" t="s">
+      <c r="E60" s="34" t="s">
         <v>374</v>
       </c>
     </row>
@@ -3746,7 +3749,7 @@
       <c r="D61" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E61" s="35"/>
+      <c r="E61" s="34"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
@@ -3756,7 +3759,7 @@
         <v>166</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="E62" s="35"/>
+      <c r="E62" s="34"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="22" t="s">
@@ -3766,7 +3769,7 @@
         <v>169</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="E63" s="35" t="s">
+      <c r="E63" s="34" t="s">
         <v>375</v>
       </c>
     </row>
@@ -3778,7 +3781,7 @@
         <v>170</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="E64" s="35"/>
+      <c r="E64" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3825,8 +3828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3862,7 +3865,7 @@
         <v>200</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>67</v>
+        <v>394</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>380</v>
@@ -3875,7 +3878,7 @@
       <c r="B3" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
@@ -3884,7 +3887,7 @@
       <c r="B4" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
@@ -3893,7 +3896,7 @@
       <c r="B5" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
@@ -3902,7 +3905,7 @@
       <c r="B6" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>383</v>
       </c>
     </row>
@@ -3913,7 +3916,7 @@
       <c r="B7" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
@@ -3944,7 +3947,7 @@
       <c r="B10" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="34" t="s">
         <v>380</v>
       </c>
     </row>
@@ -3955,7 +3958,7 @@
       <c r="B11" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
@@ -3964,7 +3967,7 @@
       <c r="B12" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
@@ -3973,7 +3976,7 @@
       <c r="B13" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3985,7 +3988,7 @@
       <c r="C14" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -4000,7 +4003,7 @@
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="30" t="s">
@@ -4012,7 +4015,7 @@
       <c r="C16" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="35"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
@@ -4021,7 +4024,7 @@
       <c r="B17" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
@@ -4030,7 +4033,7 @@
       <c r="B18" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
@@ -4076,7 +4079,7 @@
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4103,8 +4106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -4152,7 +4155,7 @@
       <c r="B3" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
@@ -4164,7 +4167,7 @@
       <c r="C4" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
@@ -4176,7 +4179,7 @@
       <c r="C5" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
@@ -4185,7 +4188,7 @@
       <c r="B6" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="35"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
@@ -4194,7 +4197,7 @@
       <c r="B7" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="34" t="s">
         <v>390</v>
       </c>
     </row>
@@ -4205,7 +4208,7 @@
       <c r="B8" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="37" t="s">
@@ -4237,7 +4240,7 @@
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -4246,7 +4249,7 @@
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
@@ -4255,7 +4258,7 @@
       <c r="B13" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="34" t="s">
         <v>386</v>
       </c>
     </row>
@@ -4266,7 +4269,7 @@
       <c r="B14" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -4275,7 +4278,7 @@
       <c r="B15" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
@@ -4284,7 +4287,7 @@
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="37" t="s">
@@ -4316,7 +4319,7 @@
       <c r="B19" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -4325,7 +4328,7 @@
       <c r="B20" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -4334,7 +4337,7 @@
       <c r="B21" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -4343,7 +4346,7 @@
       <c r="B22" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -4352,7 +4355,7 @@
       <c r="B23" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="48" t="s">
@@ -4381,7 +4384,7 @@
       <c r="B26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
modify some test and add command
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\STV-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C7056-E542-B94F-A339-F36621D2B4EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>J T</author>
   </authors>
   <commentList>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{DCA326BF-D23A-8941-AD0F-8DD6074573D4}">
+    <comment ref="H10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="396">
   <si>
     <t>component</t>
   </si>
@@ -416,7 +415,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -442,7 +441,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -545,7 +544,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -601,7 +600,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -624,7 +623,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -647,7 +646,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -670,7 +669,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -693,7 +692,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -722,7 +721,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -745,7 +744,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -878,7 +877,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -994,7 +993,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1017,7 +1016,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1040,7 +1039,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1063,7 +1062,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1137,7 +1136,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1454,7 +1453,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1476,7 +1475,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1499,7 +1498,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1522,7 +1521,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1560,7 +1559,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1583,7 +1582,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1601,7 +1600,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1639,7 +1638,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1668,7 +1667,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1694,7 +1693,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1774,18 +1773,23 @@
     <t>//*[@index='0']//*[@class='android.widget.EditText']</t>
   </si>
   <si>
-    <t>//*[@index='0' and @class='android.widget.ImageButton']</t>
+    <t>//*[@resource-id='android:id/button1']</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>//*[@index='1' and @class='android.view.ViewGroup']/*[@index='0' and @class='android.widget.ImageButton']</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1805,14 +1809,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1824,27 +1828,27 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="8" tint="0.59999389629810485"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="4"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1852,7 +1856,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1860,6 +1864,13 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2023,6 +2034,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2053,15 +2073,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2079,8 +2090,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2391,21 +2402,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="99.375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.625" style="11" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
@@ -2432,7 +2443,7 @@
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="36" t="s">
         <v>371</v>
       </c>
     </row>
@@ -2443,7 +2454,7 @@
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
@@ -2452,7 +2463,7 @@
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
@@ -2462,7 +2473,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="34"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
@@ -2472,7 +2483,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="34"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
@@ -2482,7 +2493,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="34"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
@@ -2492,7 +2503,7 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="34"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
@@ -2502,7 +2513,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="34"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
@@ -2514,7 +2525,7 @@
       <c r="C10" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
@@ -2526,7 +2537,7 @@
       <c r="C11" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
@@ -2538,16 +2549,16 @@
       <c r="C12" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
@@ -2556,7 +2567,7 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="33" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2567,7 +2578,7 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="44"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
@@ -2594,7 +2605,7 @@
       <c r="D17" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="34" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2605,7 +2616,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="44"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2614,16 +2625,16 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="45"/>
+      <c r="E19" s="35"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="40" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -2632,7 +2643,7 @@
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="36" t="s">
         <v>290</v>
       </c>
     </row>
@@ -2643,16 +2654,16 @@
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="40" t="s">
         <v>279</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
@@ -2661,7 +2672,7 @@
       <c r="B24" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="36" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2672,7 +2683,7 @@
       <c r="B25" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="E25" s="37"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
@@ -2681,7 +2692,7 @@
       <c r="B26" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="34"/>
+      <c r="E26" s="37"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
@@ -2690,16 +2701,16 @@
       <c r="B27" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E27" s="35"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
@@ -2708,7 +2719,7 @@
       <c r="B29" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="36" t="s">
         <v>292</v>
       </c>
     </row>
@@ -2719,7 +2730,7 @@
       <c r="B30" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="34"/>
+      <c r="E30" s="37"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
@@ -2728,7 +2739,7 @@
       <c r="B31" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="37"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
@@ -2737,7 +2748,7 @@
       <c r="B32" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E32" s="34"/>
+      <c r="E32" s="37"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
@@ -2749,16 +2760,16 @@
       <c r="C33" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E33" s="35"/>
+      <c r="E33" s="38"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="40" t="s">
         <v>275</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
@@ -2768,7 +2779,7 @@
         <v>258</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="36" t="s">
         <v>293</v>
       </c>
     </row>
@@ -2779,7 +2790,7 @@
       <c r="B36" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E36" s="34"/>
+      <c r="E36" s="37"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
@@ -2788,7 +2799,7 @@
       <c r="B37" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E37" s="34"/>
+      <c r="E37" s="37"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="13" t="s">
@@ -2797,7 +2808,7 @@
       <c r="B38" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E38" s="34"/>
+      <c r="E38" s="37"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
@@ -2806,7 +2817,7 @@
       <c r="B39" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E39" s="34"/>
+      <c r="E39" s="37"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
@@ -2818,16 +2829,16 @@
       <c r="C40" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E40" s="35"/>
+      <c r="E40" s="38"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="43" t="s">
         <v>276</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="42"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="45"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
@@ -2837,7 +2848,7 @@
         <v>260</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="E42" s="33" t="s">
+      <c r="E42" s="36" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2848,7 +2859,7 @@
       <c r="B43" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="E43" s="34"/>
+      <c r="E43" s="37"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -2857,7 +2868,7 @@
       <c r="B44" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="E44" s="34"/>
+      <c r="E44" s="37"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -2866,7 +2877,7 @@
       <c r="B45" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="E45" s="34"/>
+      <c r="E45" s="37"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -2878,7 +2889,7 @@
       <c r="C46" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E46" s="34"/>
+      <c r="E46" s="37"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -2890,16 +2901,16 @@
       <c r="C47" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E47" s="35"/>
+      <c r="E47" s="38"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="42"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
@@ -2909,7 +2920,7 @@
         <v>261</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="E49" s="33" t="s">
+      <c r="E49" s="36" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2920,7 +2931,7 @@
       <c r="B50" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="E50" s="34"/>
+      <c r="E50" s="37"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -2929,7 +2940,7 @@
       <c r="B51" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="E51" s="34"/>
+      <c r="E51" s="37"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
@@ -2938,7 +2949,7 @@
       <c r="B52" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="E52" s="34"/>
+      <c r="E52" s="37"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -2947,7 +2958,7 @@
       <c r="B53" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E53" s="34"/>
+      <c r="E53" s="37"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -2959,16 +2970,16 @@
       <c r="C54" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E54" s="35"/>
+      <c r="E54" s="38"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="40" t="s">
         <v>278</v>
       </c>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="39"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="42"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
@@ -2981,7 +2992,7 @@
       <c r="D56" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E56" s="33" t="s">
+      <c r="E56" s="36" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2993,7 +3004,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="E57" s="36"/>
+      <c r="E57" s="39"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3002,7 +3013,7 @@
       <c r="B58" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="E58" s="34"/>
+      <c r="E58" s="37"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3014,7 +3025,7 @@
       <c r="C59" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E59" s="34"/>
+      <c r="E59" s="37"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="14" t="s">
@@ -3026,7 +3037,7 @@
       <c r="C60" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E60" s="34"/>
+      <c r="E60" s="37"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="11" t="s">
@@ -3038,20 +3049,20 @@
       <c r="C61" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E61" s="34"/>
+      <c r="E61" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E2:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E21:E22"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
-    <mergeCell ref="E2:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E21:E22"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="E24:E27"/>
     <mergeCell ref="A34:E34"/>
@@ -3061,17 +3072,18 @@
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A55:E55"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
-    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{41B9DE7C-F513-7A4C-9608-80B8C1A2E0C8}"/>
-    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png" xr:uid="{FFDED12F-6E60-764B-AC50-E9A151FE766C}"/>
-    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png" xr:uid="{D4E49EAD-B8B9-0A49-B1A0-60F7A38DE2EA}"/>
-    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png" xr:uid="{ABDF668C-400D-2A4E-86EB-E9FD7C44BF55}"/>
-    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png" xr:uid="{DF68C727-EFA0-7542-B392-52D12BE8F88E}"/>
-    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png" xr:uid="{226D5616-AE1A-D140-B96F-B62F1F00654E}"/>
-    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png" xr:uid="{ED8A8934-31FF-2741-88B1-D7C03C047E87}"/>
-    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png" xr:uid="{152810F4-07BC-2D49-9C95-15E7C17419AF}"/>
-    <hyperlink ref="E16" r:id="rId10" xr:uid="{8E6C32E5-2FBC-974B-A364-C1B820563A7B}"/>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png"/>
+    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png"/>
+    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png"/>
+    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png"/>
+    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png"/>
+    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png"/>
+    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png"/>
+    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png"/>
+    <hyperlink ref="E16" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3079,24 +3091,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="97.83203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="11"/>
+    <col min="2" max="2" width="97.875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.625" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" customHeight="1">
+    <row r="1" spans="1:5" ht="21.95" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3166,7 +3178,7 @@
       <c r="D6" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="37" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3177,7 +3189,7 @@
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
@@ -3186,7 +3198,7 @@
       <c r="B8" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="37" t="s">
         <v>376</v>
       </c>
     </row>
@@ -3197,7 +3209,7 @@
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="34"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
@@ -3206,7 +3218,7 @@
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
@@ -3215,7 +3227,7 @@
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -3227,7 +3239,7 @@
       <c r="C12" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="37" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3241,7 +3253,7 @@
       <c r="D13" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3253,7 +3265,7 @@
       <c r="D14" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -3268,7 +3280,7 @@
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
@@ -3280,7 +3292,7 @@
       <c r="C16" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -3289,7 +3301,7 @@
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -3298,7 +3310,7 @@
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="37"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -3307,7 +3319,7 @@
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -3316,7 +3328,7 @@
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="37"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -3325,7 +3337,7 @@
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="37"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -3334,7 +3346,7 @@
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="37"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -3343,7 +3355,7 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="34" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3354,7 +3366,7 @@
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="44"/>
+      <c r="E24" s="34"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
@@ -3380,7 +3392,7 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="34" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3391,7 +3403,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="44"/>
+      <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3400,7 +3412,7 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="44"/>
+      <c r="E28" s="34"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
@@ -3409,7 +3421,7 @@
       <c r="B29" s="28" t="s">
         <v>392</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="34"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
@@ -3418,7 +3430,7 @@
       <c r="B30" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="E30" s="44"/>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3427,7 +3439,7 @@
       <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="37" t="s">
         <v>377</v>
       </c>
     </row>
@@ -3438,7 +3450,7 @@
       <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="34"/>
+      <c r="E32" s="37"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3447,7 +3459,7 @@
       <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E33" s="34"/>
+      <c r="E33" s="37"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
@@ -3456,7 +3468,7 @@
       <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="34"/>
+      <c r="E34" s="37"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
@@ -3476,7 +3488,7 @@
       <c r="B36" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="37" t="s">
         <v>378</v>
       </c>
     </row>
@@ -3487,7 +3499,7 @@
       <c r="B37" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="34"/>
+      <c r="E37" s="37"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3496,7 +3508,7 @@
       <c r="B38" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="34"/>
+      <c r="E38" s="37"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="22" t="s">
@@ -3505,7 +3517,7 @@
       <c r="B39" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="34"/>
+      <c r="E39" s="37"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
@@ -3522,13 +3534,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
@@ -3538,7 +3550,7 @@
         <v>73</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="E42" s="33" t="s">
+      <c r="E42" s="36" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3550,7 +3562,7 @@
         <v>74</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="34"/>
+      <c r="E43" s="37"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -3560,7 +3572,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="34"/>
+      <c r="E44" s="37"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -3570,7 +3582,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="34"/>
+      <c r="E45" s="37"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -3580,7 +3592,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="34"/>
+      <c r="E46" s="37"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -3590,7 +3602,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="E47" s="34"/>
+      <c r="E47" s="37"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
@@ -3602,7 +3614,7 @@
       <c r="C48" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="E48" s="34"/>
+      <c r="E48" s="37"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="11" t="s">
@@ -3619,13 +3631,13 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="39"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="42"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -3635,7 +3647,7 @@
         <v>73</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="E51" s="33" t="s">
+      <c r="E51" s="36" t="s">
         <v>373</v>
       </c>
     </row>
@@ -3647,7 +3659,7 @@
         <v>74</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="E52" s="34"/>
+      <c r="E52" s="37"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -3657,7 +3669,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="E53" s="34"/>
+      <c r="E53" s="37"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -3667,7 +3679,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="E54" s="34"/>
+      <c r="E54" s="37"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
@@ -3677,7 +3689,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="E55" s="34"/>
+      <c r="E55" s="37"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="11" t="s">
@@ -3689,7 +3701,7 @@
       <c r="C56" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="E56" s="34"/>
+      <c r="E56" s="37"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
@@ -3701,7 +3713,7 @@
       <c r="C57" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="E57" s="34"/>
+      <c r="E57" s="37"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3711,7 +3723,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="E58" s="34"/>
+      <c r="E58" s="37"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3721,7 +3733,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="E59" s="34"/>
+      <c r="E59" s="37"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="13" t="s">
@@ -3734,7 +3746,7 @@
       <c r="D60" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E60" s="34" t="s">
+      <c r="E60" s="37" t="s">
         <v>374</v>
       </c>
     </row>
@@ -3749,7 +3761,7 @@
       <c r="D61" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E61" s="34"/>
+      <c r="E61" s="37"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
@@ -3759,7 +3771,7 @@
         <v>166</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="E62" s="34"/>
+      <c r="E62" s="37"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="22" t="s">
@@ -3769,7 +3781,7 @@
         <v>169</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="E63" s="34" t="s">
+      <c r="E63" s="37" t="s">
         <v>375</v>
       </c>
     </row>
@@ -3781,7 +3793,7 @@
         <v>170</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="E64" s="34"/>
+      <c r="E64" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3800,24 +3812,25 @@
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="E12:E22"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{9FE2AE8E-A9CA-964E-A11C-56069919D277}"/>
-    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{AF945763-504F-F44B-941F-F68473F43173}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{C90C6E02-C85B-3048-B0C9-FEDCC070B8E1}"/>
-    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{7200B3E4-19A9-E34E-B217-AC9A8F0454BD}"/>
-    <hyperlink ref="E35" r:id="rId5" xr:uid="{8446D4E4-077D-0A4D-8525-8FB07FF0C373}"/>
-    <hyperlink ref="E40" r:id="rId6" xr:uid="{12FBB57A-780E-814C-87D8-AFBFE84831F1}"/>
-    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png" xr:uid="{610945C3-6CA0-044C-8FF8-83DD72D73D6A}"/>
-    <hyperlink ref="E49" r:id="rId8" xr:uid="{7E1BB3A1-2AEF-CA43-9C3D-463F6622F876}"/>
-    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png" xr:uid="{AAD316A3-DB94-4240-B398-3FB32A25F9D3}"/>
-    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png" xr:uid="{17A3A39B-02B6-714F-9B1B-FD402BDF5ABA}"/>
-    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png" xr:uid="{AB6376ED-61CD-AD4E-B9AC-DB5009AA4A5C}"/>
-    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png" xr:uid="{727B6477-B8DF-D142-8C44-57DAF56E23D5}"/>
-    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png" xr:uid="{FDC259CA-E4C3-6746-98E2-92665C5A49E4}"/>
-    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png" xr:uid="{D0EA7266-482F-8D4F-8F27-B9084ABDA77D}"/>
-    <hyperlink ref="E25" r:id="rId15" xr:uid="{ACC8DD5A-7237-0E49-90A1-C93B1602CF73}"/>
-    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png" xr:uid="{E529EFF7-B7A1-524E-A663-6A19E3F92017}"/>
-    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png" xr:uid="{1A63B7F9-20A8-9A47-844C-ED1A1163AB29}"/>
+    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png"/>
+    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png"/>
+    <hyperlink ref="E35" r:id="rId5"/>
+    <hyperlink ref="E40" r:id="rId6"/>
+    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png"/>
+    <hyperlink ref="E49" r:id="rId8"/>
+    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png"/>
+    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png"/>
+    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png"/>
+    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png"/>
+    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png"/>
+    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png"/>
+    <hyperlink ref="E25" r:id="rId15"/>
+    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png"/>
+    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3825,22 +3838,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="28.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="123.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="31.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="31.125" style="11" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="11"/>
+    <col min="7" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3865,9 +3878,9 @@
         <v>200</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>394</v>
-      </c>
-      <c r="E2" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" s="36" t="s">
         <v>380</v>
       </c>
     </row>
@@ -3878,7 +3891,7 @@
       <c r="B3" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
@@ -3887,7 +3900,7 @@
       <c r="B4" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
@@ -3896,7 +3909,7 @@
       <c r="B5" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
@@ -3905,7 +3918,7 @@
       <c r="B6" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="37" t="s">
         <v>383</v>
       </c>
     </row>
@@ -3916,7 +3929,7 @@
       <c r="B7" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
@@ -3947,7 +3960,7 @@
       <c r="B10" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="37" t="s">
         <v>380</v>
       </c>
     </row>
@@ -3958,7 +3971,7 @@
       <c r="B11" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
@@ -3967,7 +3980,7 @@
       <c r="B12" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
@@ -3976,7 +3989,7 @@
       <c r="B13" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3988,7 +4001,7 @@
       <c r="C14" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -4003,7 +4016,7 @@
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="30" t="s">
@@ -4015,7 +4028,7 @@
       <c r="C16" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
@@ -4024,7 +4037,7 @@
       <c r="B17" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
@@ -4033,7 +4046,7 @@
       <c r="B18" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="37"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
@@ -4066,9 +4079,9 @@
         <v>334</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="E21" s="36" t="s">
         <v>382</v>
       </c>
     </row>
@@ -4079,7 +4092,7 @@
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4089,13 +4102,14 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="E10:E18"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png" xr:uid="{DBDAF80C-9383-FC40-B83E-398C0807592C}"/>
-    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png" xr:uid="{B769E664-C3A5-C846-8710-7122F377D25C}"/>
-    <hyperlink ref="E19" r:id="rId3" xr:uid="{C5D88C3A-F299-6B4E-A9FD-59313F307545}"/>
-    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png" xr:uid="{4DF7ABBB-AA92-2E44-9C4D-E9A866C1708E}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{FFBC2EC3-5D16-8D4F-B3A3-FD8D1BDC8A1D}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{5752B374-7244-E240-924D-FA39114A1383}"/>
+    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png"/>
+    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png"/>
+    <hyperlink ref="E19" r:id="rId3"/>
+    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png"/>
+    <hyperlink ref="E9" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4103,21 +4117,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="27.625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="113.625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="23.375" style="11" customWidth="1"/>
     <col min="4" max="4" width="14" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4144,7 +4158,7 @@
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="36" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4155,7 +4169,7 @@
       <c r="B3" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
@@ -4167,7 +4181,7 @@
       <c r="C4" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
@@ -4179,7 +4193,7 @@
       <c r="C5" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
@@ -4188,7 +4202,7 @@
       <c r="B6" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
@@ -4197,7 +4211,7 @@
       <c r="B7" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="37" t="s">
         <v>390</v>
       </c>
     </row>
@@ -4208,16 +4222,16 @@
       <c r="B8" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="40" t="s">
         <v>285</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
@@ -4229,7 +4243,7 @@
       <c r="D10" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="36" t="s">
         <v>388</v>
       </c>
     </row>
@@ -4240,7 +4254,7 @@
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -4249,7 +4263,7 @@
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
@@ -4258,7 +4272,7 @@
       <c r="B13" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="37" t="s">
         <v>386</v>
       </c>
     </row>
@@ -4269,7 +4283,7 @@
       <c r="B14" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -4278,7 +4292,7 @@
       <c r="B15" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
@@ -4287,16 +4301,16 @@
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="35"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -4308,7 +4322,7 @@
       <c r="C18" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="36" t="s">
         <v>391</v>
       </c>
     </row>
@@ -4319,7 +4333,7 @@
       <c r="B19" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -4328,7 +4342,7 @@
       <c r="B20" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="37"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -4337,7 +4351,7 @@
       <c r="B21" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="37"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -4346,7 +4360,7 @@
       <c r="B22" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="37"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -4355,7 +4369,7 @@
       <c r="B23" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="E23" s="35"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="48" t="s">
@@ -4373,7 +4387,7 @@
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="36" t="s">
         <v>389</v>
       </c>
     </row>
@@ -4384,7 +4398,7 @@
       <c r="B26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="34"/>
+      <c r="E26" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4398,40 +4412,41 @@
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A24:E24"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png" xr:uid="{1518F90C-C848-0E46-88B7-B89C8E1E7D4F}"/>
-    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png" xr:uid="{F7868AFA-E3A6-B44F-AABF-FEA46C17919B}"/>
-    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png" xr:uid="{C73A2777-D611-CD43-B9B4-C3594113B832}"/>
-    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png" xr:uid="{BC8B5071-BD9D-AA4A-8E01-D45B59CDDA17}"/>
-    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png" xr:uid="{BC664D47-EA3F-AC44-98C4-CB0A219B6118}"/>
-    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png" xr:uid="{BC31547B-6FE5-0843-A8E3-700C667AFBF5}"/>
+    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png"/>
+    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png"/>
+    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png"/>
+    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png"/>
+    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png"/>
+    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9A35-BE5A-E64F-9080-864E7183DD30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="107.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="31.375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="107.625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20.125" style="11" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="40" style="11" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="35.1640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="11"/>
+    <col min="6" max="6" width="20.375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="36.625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="35.125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="21.625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="21.375" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1">
@@ -4677,11 +4692,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4804,11 +4819,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -5231,12 +5246,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="39"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="42"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5317,12 +5332,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="39"/>
+      <c r="B68" s="41"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="42"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5473,10 +5488,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="37"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="39"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="41"/>
+      <c r="C83" s="41"/>
+      <c r="D83" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5486,8 +5501,9 @@
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A13:C13"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify test data for correcting ambiguous xpath of search page folder
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\STV-Project\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78BEB8-C586-7A4B-9269-845711C9B5DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -31,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J T</author>
   </authors>
   <commentList>
-    <comment ref="H10" authorId="0" shapeId="0">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="395">
   <si>
     <t>component</t>
   </si>
@@ -415,7 +416,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -441,7 +442,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -544,7 +545,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -600,7 +601,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -623,7 +624,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -646,7 +647,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -669,7 +670,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -692,7 +693,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -721,7 +722,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -744,7 +745,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -861,6 +862,99 @@
   </si>
   <si>
     <t>//*[@text='not specified']</t>
+  </si>
+  <si>
+    <t>Input field</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>return_btn</t>
+  </si>
+  <si>
+    <t>pin_task_btn</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/pin_task']</t>
+  </si>
+  <si>
+    <t>edit_btn</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/edit_task']</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/floating_action_button']</t>
+  </si>
+  <si>
+    <t>float_done_btn</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/button_add_one_day']</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/button_add_one_hour']</t>
+  </si>
+  <si>
+    <t>location_link</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.ImageView' and @index='2']</t>
+  </si>
+  <si>
+    <t>check_list_drag_handle</t>
+  </si>
+  <si>
+    <t>check_list_remove</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/remove_item']</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/add_item']</t>
+  </si>
+  <si>
+    <t>check_list_add_item</t>
+  </si>
+  <si>
+    <t>URL_link</t>
+  </si>
+  <si>
+    <t>//*[@text='Delete task']</t>
+  </si>
+  <si>
+    <t>//*[@text='Send to']</t>
+  </si>
+  <si>
+    <t>cancel_btn</t>
+  </si>
+  <si>
+    <t>//*[@text='Create Task']</t>
+  </si>
+  <si>
+    <t>//*[@text='See all']</t>
+  </si>
+  <si>
+    <t>//*[@text='Displayed Lists']</t>
+  </si>
+  <si>
+    <t>//*[@text='Settings']</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.LinearLayout' and @index='2']</t>
+  </si>
+  <si>
+    <t>//*[@text='Refresh']</t>
+  </si>
+  <si>
+    <t>add_list_btn</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/action_add_local_list']</t>
   </si>
   <si>
     <r>
@@ -877,7 +971,8 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="新細明體"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -885,101 +980,445 @@
     </r>
   </si>
   <si>
-    <t>Input field</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>return_btn</t>
-  </si>
-  <si>
-    <t>pin_task_btn</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/pin_task']</t>
-  </si>
-  <si>
-    <t>edit_btn</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/edit_task']</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/floating_action_button']</t>
-  </si>
-  <si>
-    <t>float_done_btn</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/button_add_one_day']</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/button_add_one_hour']</t>
-  </si>
-  <si>
-    <t>location_link</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.ImageView' and @index='2']</t>
-  </si>
-  <si>
-    <t>check_list_drag_handle</t>
-  </si>
-  <si>
-    <t>check_list_remove</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/remove_item']</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/add_item']</t>
-  </si>
-  <si>
-    <t>check_list_add_item</t>
-  </si>
-  <si>
-    <t>URL_link</t>
-  </si>
-  <si>
-    <t>//*[@text='Delete task']</t>
-  </si>
-  <si>
-    <t>//*[@text='Send to']</t>
-  </si>
-  <si>
-    <t>cancel_btn</t>
-  </si>
-  <si>
-    <t>//*[@text='Create Task']</t>
-  </si>
-  <si>
-    <t>//*[@text='See all']</t>
-  </si>
-  <si>
-    <t>//*[@text='Displayed Lists']</t>
-  </si>
-  <si>
-    <t>//*[@text='Settings']</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.LinearLayout' and @index='2']</t>
-  </si>
-  <si>
-    <t>//*[@text='Refresh']</t>
-  </si>
-  <si>
-    <t>add_list_btn</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/action_add_local_list']</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[@text='</t>
+    <r>
+      <t>//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']//*[@resource-id='android:id/checkbox']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']//*[@resource-id='android:id/title']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']//*[@resource-id='org.dmfs.tasks:id/drag_handle']</t>
+    </r>
+  </si>
+  <si>
+    <t>folder_setting</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/synced_task_list_button']</t>
+  </si>
+  <si>
+    <t>synchronized_lists</t>
+  </si>
+  <si>
+    <t>list_editText</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/name_setting']</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/color_setting']</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='android:id/button3']</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.ImageView' and @index='3']</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.ImageView' and @index='4']</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.ImageView' and @index='5']</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.ImageView' and @index='6']</t>
+  </si>
+  <si>
+    <t>color_set_1</t>
+  </si>
+  <si>
+    <t>color_set_2</t>
+  </si>
+  <si>
+    <t>color_set_3</t>
+  </si>
+  <si>
+    <t>color_set_4</t>
+  </si>
+  <si>
+    <t>color_set_5</t>
+  </si>
+  <si>
+    <t>pick_color</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.GridView']//*[@class='android.widget.LinearLayout' and @index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']</t>
+    </r>
+  </si>
+  <si>
+    <t>synchronized_cancel</t>
+  </si>
+  <si>
+    <t>synchronized_ok</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.Button' and @text='CANCEL']</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.Button' and @text='OK']</t>
+  </si>
+  <si>
+    <t>//*[@text='Today']</t>
+  </si>
+  <si>
+    <t>//*[@text='Tomorrow']</t>
+  </si>
+  <si>
+    <t>//*[@text='Next days']</t>
+  </si>
+  <si>
+    <t>//*[@text='Someday']</t>
+  </si>
+  <si>
+    <t>//*[@text='Already Started']</t>
+  </si>
+  <si>
+    <t>//*[@text='Later']</t>
+  </si>
+  <si>
+    <t>//*[@text='High priority']</t>
+  </si>
+  <si>
+    <t>//*[@text='Almost done']</t>
+  </si>
+  <si>
+    <t>//*[@text='Halfway there']</t>
+  </si>
+  <si>
+    <t>//*[@text='Way to go']</t>
+  </si>
+  <si>
+    <t>//*[@text='Nothing accomplished']</t>
+  </si>
+  <si>
+    <t>//*[@text='Done']</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/search_src_text']</t>
+  </si>
+  <si>
+    <t>search_editText</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/search_close_btn']</t>
+  </si>
+  <si>
+    <t>quick add</t>
+  </si>
+  <si>
+    <t>input field</t>
+  </si>
+  <si>
+    <t>calendar</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>menu_btn</t>
+  </si>
+  <si>
+    <t>task due</t>
+  </si>
+  <si>
+    <t>task starting</t>
+  </si>
+  <si>
+    <t>task priority</t>
+  </si>
+  <si>
+    <t>task progress</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>menu_displayed_lists</t>
+  </si>
+  <si>
+    <t>menu_settings</t>
+  </si>
+  <si>
+    <t>menu_show_completed_tasks</t>
+  </si>
+  <si>
+    <t>menu_refresh</t>
+  </si>
+  <si>
+    <t>confirm delete</t>
+  </si>
+  <si>
+    <t>edit lists' information</t>
+  </si>
+  <si>
+    <t>color setting</t>
+  </si>
+  <si>
+    <t>status_dropdown</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>QuickAdd.png</t>
+  </si>
+  <si>
+    <t>ConfirmDelete.png</t>
+  </si>
+  <si>
+    <t>TaskListMenu.png</t>
+  </si>
+  <si>
+    <t>TasksDue.png</t>
+  </si>
+  <si>
+    <t>TasksStarting.png</t>
+  </si>
+  <si>
+    <t>TasksPriority.png</t>
+  </si>
+  <si>
+    <t>TaskProgress.png</t>
+  </si>
+  <si>
+    <t>remove_record_btn</t>
+  </si>
+  <si>
+    <t>search_back_btn</t>
+  </si>
+  <si>
+    <t>Search.png</t>
+  </si>
+  <si>
+    <t>priority_dropdown</t>
+  </si>
+  <si>
+    <t>privacy_dropdown</t>
+  </si>
+  <si>
+    <t>time_zone_dropdown</t>
+  </si>
+  <si>
+    <t>EditTask1.png</t>
+  </si>
+  <si>
+    <t>folder_dropdown</t>
+  </si>
+  <si>
+    <t>FolderOptions.png</t>
+  </si>
+  <si>
+    <t>EditTask2.png</t>
+  </si>
+  <si>
+    <t>Calendar.png</t>
+  </si>
+  <si>
+    <t>CalendarPickYear.png</t>
+  </si>
+  <si>
+    <t>calendar_ok_btn</t>
+  </si>
+  <si>
+    <t>calendar_cancel_btn</t>
+  </si>
+  <si>
+    <t>time_ok_btn</t>
+  </si>
+  <si>
+    <t>time_cancel_btn</t>
+  </si>
+  <si>
+    <t>time_AMPM_dropdown</t>
+  </si>
+  <si>
+    <t>today_folder</t>
+  </si>
+  <si>
+    <t>tomorrow_folder</t>
+  </si>
+  <si>
+    <t>next_days_folder</t>
+  </si>
+  <si>
+    <t>someday_folder</t>
+  </si>
+  <si>
+    <t>already_started_folder</t>
+  </si>
+  <si>
+    <t>later_folder</t>
+  </si>
+  <si>
+    <t>high_priority_folder</t>
+  </si>
+  <si>
+    <t>medium_priority_folder</t>
+  </si>
+  <si>
+    <t>low_priority_folder</t>
+  </si>
+  <si>
+    <t>no_priority_folder</t>
+  </si>
+  <si>
+    <t>almost_done_folder</t>
+  </si>
+  <si>
+    <t>halfway_there_folder</t>
+  </si>
+  <si>
+    <t>way_to_go_folder</t>
+  </si>
+  <si>
+    <t>nothing_accomplished_folder</t>
+  </si>
+  <si>
+    <t>done_folder</t>
+  </si>
+  <si>
+    <t>menu_delete_btn</t>
+  </si>
+  <si>
+    <t>menu_send_to_btn</t>
+  </si>
+  <si>
+    <t>menu_create_teask_btn</t>
+  </si>
+  <si>
+    <t>menu_see_all_btn</t>
+  </si>
+  <si>
+    <t>+1day_btn</t>
+  </si>
+  <si>
+    <t>+1hour_btn</t>
+  </si>
+  <si>
+    <t>confirm_delete_ok_btn</t>
+  </si>
+  <si>
+    <t>confirm_delete_cancel_btn</t>
+  </si>
+  <si>
+    <t>list_ok_btn</t>
+  </si>
+  <si>
+    <t>list_cancel_btn</t>
+  </si>
+  <si>
+    <t>list_name_setting</t>
+  </si>
+  <si>
+    <t>list_color_setting</t>
+  </si>
+  <si>
+    <t>list_save_btn</t>
+  </si>
+  <si>
+    <t>list_delete_list_btn</t>
+  </si>
+  <si>
+    <t>${NAME}</t>
+  </si>
+  <si>
+    <t>${INDEX}</t>
+  </si>
+  <si>
+    <t>${HOURS}</t>
+  </si>
+  <si>
+    <t>${MINUTES}</t>
+  </si>
+  <si>
+    <t>${DATE}</t>
+  </si>
+  <si>
+    <t>${YEAR}</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.LinearLayout' and ./android.widget.TextView[@text='</t>
     </r>
     <r>
       <rPr>
@@ -993,7 +1432,29 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.TextView' and @text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1002,7 +1463,7 @@
   </si>
   <si>
     <r>
-      <t>//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
     </r>
     <r>
       <rPr>
@@ -1015,17 +1476,17 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>']//*[@resource-id='android:id/checkbox']</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+      <t>']//*[@resource-id='android:id/text1']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
     </r>
     <r>
       <rPr>
@@ -1038,17 +1499,166 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>']//*[@resource-id='android:id/title']</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+      <t>']//*[@resource-id='android:id/checkbox']</t>
+    </r>
+  </si>
+  <si>
+    <t>//*[@index='11']//*[@class='android.widget.Spinner']</t>
+  </si>
+  <si>
+    <t>//*[@text='needs action']</t>
+  </si>
+  <si>
+    <t>//*[@index='12']//*[@class='android.widget.Spinner']</t>
+  </si>
+  <si>
+    <t>//*[@index='13']//*[@class='android.widget.EditText']</t>
+  </si>
+  <si>
+    <t>time_zone_options</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.LinearLayout']//*[contains(@text, '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>') and @resource-id='org.dmfs.tasks:id/integer_choice_item_text']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>android.widget.LinearLayout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' and ./android.widget.TextView[@text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']]</t>
+    </r>
+  </si>
+  <si>
+    <t>partial name acceptable</t>
+  </si>
+  <si>
+    <t>//*[@text='Medium priority']</t>
+  </si>
+  <si>
+    <t>//*[@text='Low priority']</t>
+  </si>
+  <si>
+    <t>//*[@text='No priority']</t>
+  </si>
+  <si>
+    <t>search_clear_btn</t>
+  </si>
+  <si>
+    <r>
+      <t>//*/android.widget.FrameLayout/android.widget.RelativeLayout//*[@text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']</t>
+    </r>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/content']//*[@class='android.widget.LinearLayout' and @index='1']</t>
+  </si>
+  <si>
+    <t>${URL}</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[contains(@text, '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${URL}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>')]</t>
+    </r>
+  </si>
+  <si>
+    <t>partial url</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.RelativeLayout' and @index='</t>
     </r>
     <r>
       <rPr>
@@ -1062,638 +1672,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']//*[@resource-id='org.dmfs.tasks:id/drag_handle']</t>
-    </r>
-  </si>
-  <si>
-    <t>folder_setting</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/synced_task_list_button']</t>
-  </si>
-  <si>
-    <t>synchronized_lists</t>
-  </si>
-  <si>
-    <t>list_editText</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/name_setting']</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/color_setting']</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='android:id/button3']</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.ImageView' and @index='3']</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.ImageView' and @index='4']</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.ImageView' and @index='5']</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.ImageView' and @index='6']</t>
-  </si>
-  <si>
-    <t>color_set_1</t>
-  </si>
-  <si>
-    <t>color_set_2</t>
-  </si>
-  <si>
-    <t>color_set_3</t>
-  </si>
-  <si>
-    <t>color_set_4</t>
-  </si>
-  <si>
-    <t>color_set_5</t>
-  </si>
-  <si>
-    <t>pick_color</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='android.widget.GridView']//*[@class='android.widget.LinearLayout' and @index='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${INDEX}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']</t>
-    </r>
-  </si>
-  <si>
-    <t>synchronized_cancel</t>
-  </si>
-  <si>
-    <t>synchronized_ok</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.Button' and @text='CANCEL']</t>
-  </si>
-  <si>
-    <t>//*[@class='android.widget.Button' and @text='OK']</t>
-  </si>
-  <si>
-    <t>//*[@text='Today']</t>
-  </si>
-  <si>
-    <t>//*[@text='Tomorrow']</t>
-  </si>
-  <si>
-    <t>//*[@text='Next days']</t>
-  </si>
-  <si>
-    <t>//*[@text='Someday']</t>
-  </si>
-  <si>
-    <t>//*[@text='Already Started']</t>
-  </si>
-  <si>
-    <t>//*[@text='Later']</t>
-  </si>
-  <si>
-    <t>//*[@text='High priority']</t>
-  </si>
-  <si>
-    <t>//*[@text='Almost done']</t>
-  </si>
-  <si>
-    <t>//*[@text='Halfway there']</t>
-  </si>
-  <si>
-    <t>//*[@text='Way to go']</t>
-  </si>
-  <si>
-    <t>//*[@text='Nothing accomplished']</t>
-  </si>
-  <si>
-    <t>//*[@text='Done']</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/search_src_text']</t>
-  </si>
-  <si>
-    <t>search_editText</t>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/search_close_btn']</t>
-  </si>
-  <si>
-    <t>quick add</t>
-  </si>
-  <si>
-    <t>input field</t>
-  </si>
-  <si>
-    <t>calendar</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>menu_btn</t>
-  </si>
-  <si>
-    <t>task due</t>
-  </si>
-  <si>
-    <t>task starting</t>
-  </si>
-  <si>
-    <t>task priority</t>
-  </si>
-  <si>
-    <t>task progress</t>
-  </si>
-  <si>
-    <t>search</t>
-  </si>
-  <si>
-    <t>menu</t>
-  </si>
-  <si>
-    <t>menu_displayed_lists</t>
-  </si>
-  <si>
-    <t>menu_settings</t>
-  </si>
-  <si>
-    <t>menu_show_completed_tasks</t>
-  </si>
-  <si>
-    <t>menu_refresh</t>
-  </si>
-  <si>
-    <t>confirm delete</t>
-  </si>
-  <si>
-    <t>edit lists' information</t>
-  </si>
-  <si>
-    <t>color setting</t>
-  </si>
-  <si>
-    <t>status_dropdown</t>
-  </si>
-  <si>
-    <t>reference</t>
-  </si>
-  <si>
-    <t>QuickAdd.png</t>
-  </si>
-  <si>
-    <t>ConfirmDelete.png</t>
-  </si>
-  <si>
-    <t>TaskListMenu.png</t>
-  </si>
-  <si>
-    <t>TasksDue.png</t>
-  </si>
-  <si>
-    <t>TasksStarting.png</t>
-  </si>
-  <si>
-    <t>TasksPriority.png</t>
-  </si>
-  <si>
-    <t>TaskProgress.png</t>
-  </si>
-  <si>
-    <t>remove_record_btn</t>
-  </si>
-  <si>
-    <t>search_back_btn</t>
-  </si>
-  <si>
-    <t>Search.png</t>
-  </si>
-  <si>
-    <t>priority_dropdown</t>
-  </si>
-  <si>
-    <t>privacy_dropdown</t>
-  </si>
-  <si>
-    <t>time_zone_dropdown</t>
-  </si>
-  <si>
-    <t>EditTask1.png</t>
-  </si>
-  <si>
-    <t>folder_dropdown</t>
-  </si>
-  <si>
-    <t>FolderOptions.png</t>
-  </si>
-  <si>
-    <t>EditTask2.png</t>
-  </si>
-  <si>
-    <t>Calendar.png</t>
-  </si>
-  <si>
-    <t>CalendarPickYear.png</t>
-  </si>
-  <si>
-    <t>calendar_ok_btn</t>
-  </si>
-  <si>
-    <t>calendar_cancel_btn</t>
-  </si>
-  <si>
-    <t>time_ok_btn</t>
-  </si>
-  <si>
-    <t>time_cancel_btn</t>
-  </si>
-  <si>
-    <t>time_AMPM_dropdown</t>
-  </si>
-  <si>
-    <t>today_folder</t>
-  </si>
-  <si>
-    <t>tomorrow_folder</t>
-  </si>
-  <si>
-    <t>next_days_folder</t>
-  </si>
-  <si>
-    <t>someday_folder</t>
-  </si>
-  <si>
-    <t>already_started_folder</t>
-  </si>
-  <si>
-    <t>later_folder</t>
-  </si>
-  <si>
-    <t>high_priority_folder</t>
-  </si>
-  <si>
-    <t>medium_priority_folder</t>
-  </si>
-  <si>
-    <t>low_priority_folder</t>
-  </si>
-  <si>
-    <t>no_priority_folder</t>
-  </si>
-  <si>
-    <t>almost_done_folder</t>
-  </si>
-  <si>
-    <t>halfway_there_folder</t>
-  </si>
-  <si>
-    <t>way_to_go_folder</t>
-  </si>
-  <si>
-    <t>nothing_accomplished_folder</t>
-  </si>
-  <si>
-    <t>done_folder</t>
-  </si>
-  <si>
-    <t>menu_delete_btn</t>
-  </si>
-  <si>
-    <t>menu_send_to_btn</t>
-  </si>
-  <si>
-    <t>menu_create_teask_btn</t>
-  </si>
-  <si>
-    <t>menu_see_all_btn</t>
-  </si>
-  <si>
-    <t>+1day_btn</t>
-  </si>
-  <si>
-    <t>+1hour_btn</t>
-  </si>
-  <si>
-    <t>confirm_delete_ok_btn</t>
-  </si>
-  <si>
-    <t>confirm_delete_cancel_btn</t>
-  </si>
-  <si>
-    <t>list_ok_btn</t>
-  </si>
-  <si>
-    <t>list_cancel_btn</t>
-  </si>
-  <si>
-    <t>list_name_setting</t>
-  </si>
-  <si>
-    <t>list_color_setting</t>
-  </si>
-  <si>
-    <t>list_save_btn</t>
-  </si>
-  <si>
-    <t>list_delete_list_btn</t>
-  </si>
-  <si>
-    <t>${NAME}</t>
-  </si>
-  <si>
-    <t>${INDEX}</t>
-  </si>
-  <si>
-    <t>${HOURS}</t>
-  </si>
-  <si>
-    <t>${MINUTES}</t>
-  </si>
-  <si>
-    <t>${DATE}</t>
-  </si>
-  <si>
-    <t>${YEAR}</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='android.widget.LinearLayout' and ./android.widget.TextView[@text='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${NAME}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='android.widget.TextView' and @text='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${NAME}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${INDEX}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']//*[@resource-id='android:id/text1']</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${INDEX}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']//*[@resource-id='android:id/checkbox']</t>
-    </r>
-  </si>
-  <si>
-    <t>//*[@index='11']//*[@class='android.widget.Spinner']</t>
-  </si>
-  <si>
-    <t>//*[@text='needs action']</t>
-  </si>
-  <si>
-    <t>//*[@index='12']//*[@class='android.widget.Spinner']</t>
-  </si>
-  <si>
-    <t>//*[@index='13']//*[@class='android.widget.EditText']</t>
-  </si>
-  <si>
-    <t>time_zone_options</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='android.widget.LinearLayout']//*[contains(@text, '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${NAME}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>') and @resource-id='org.dmfs.tasks:id/integer_choice_item_text']</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>android.widget.LinearLayout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' and ./android.widget.TextView[@text='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${NAME}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']]</t>
-    </r>
-  </si>
-  <si>
-    <t>partial name acceptable</t>
-  </si>
-  <si>
-    <t>//*[@text='Medium priority']</t>
-  </si>
-  <si>
-    <t>//*[@text='Low priority']</t>
-  </si>
-  <si>
-    <t>//*[@text='No priority']</t>
-  </si>
-  <si>
-    <t>search_clear_btn</t>
-  </si>
-  <si>
-    <r>
-      <t>//*/android.widget.FrameLayout/android.widget.RelativeLayout//*[@text='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${NAME}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']</t>
-    </r>
-  </si>
-  <si>
-    <t>//*[@resource-id='org.dmfs.tasks:id/content']//*[@class='android.widget.LinearLayout' and @index='1']</t>
-  </si>
-  <si>
-    <t>${URL}</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[contains(@text, '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${URL}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>')]</t>
-    </r>
-  </si>
-  <si>
-    <t>partial url</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='android.widget.RelativeLayout' and @index='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${INDEX}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1784,12 +1763,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1809,14 +1788,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1828,27 +1807,27 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="8" tint="0.59999389629810485"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="4"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1856,7 +1835,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1867,7 +1846,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2034,15 +2013,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2050,9 +2020,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2063,6 +2030,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2090,8 +2069,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2402,21 +2381,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="99.375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="11"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
@@ -2430,10 +2409,10 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2443,8 +2422,8 @@
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>371</v>
+      <c r="E2" s="33" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2454,7 +2433,7 @@
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
@@ -2463,7 +2442,7 @@
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="37"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
@@ -2473,7 +2452,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="37"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
@@ -2483,7 +2462,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="37"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
@@ -2493,7 +2472,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="37"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
@@ -2503,29 +2482,29 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="37"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="37"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E10" s="37"/>
+        <v>341</v>
+      </c>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
@@ -2535,30 +2514,30 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="E11" s="37"/>
+        <v>342</v>
+      </c>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E12" s="38"/>
+        <v>341</v>
+      </c>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
+      <c r="A13" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
@@ -2567,8 +2546,8 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="33" t="s">
-        <v>289</v>
+      <c r="E14" s="39" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2578,20 +2557,20 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F16" s="31"/>
     </row>
@@ -2603,10 +2582,10 @@
         <v>72</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>289</v>
+        <v>198</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2616,7 +2595,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2625,215 +2604,215 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="40" t="s">
-        <v>284</v>
-      </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
+      <c r="A20" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="36" t="s">
-        <v>290</v>
+      <c r="E21" s="33" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="38"/>
+      <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="40" t="s">
-        <v>279</v>
-      </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="42"/>
+      <c r="A23" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>291</v>
+        <v>221</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="E25" s="37"/>
+        <v>222</v>
+      </c>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" s="37"/>
+        <v>223</v>
+      </c>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="E27" s="38"/>
+        <v>224</v>
+      </c>
+      <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="42"/>
+      <c r="A28" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E29" s="36" t="s">
-        <v>292</v>
+        <v>253</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E30" s="37"/>
+        <v>254</v>
+      </c>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E31" s="37"/>
+        <v>255</v>
+      </c>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E32" s="37"/>
+        <v>256</v>
+      </c>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E33" s="38"/>
+        <v>341</v>
+      </c>
+      <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="40" t="s">
-        <v>275</v>
-      </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="42"/>
+      <c r="A34" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="38"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="E35" s="36" t="s">
-        <v>293</v>
+      <c r="E35" s="33" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E36" s="37"/>
+        <v>253</v>
+      </c>
+      <c r="E36" s="34"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E37" s="37"/>
+        <v>254</v>
+      </c>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E38" s="37"/>
+        <v>256</v>
+      </c>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="E39" s="37"/>
+        <v>258</v>
+      </c>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E40" s="38"/>
+        <v>341</v>
+      </c>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B41" s="44"/>
       <c r="C41" s="44"/>
@@ -2842,42 +2821,42 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="E42" s="36" t="s">
-        <v>294</v>
+      <c r="E42" s="33" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="E43" s="37"/>
+        <v>359</v>
+      </c>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="E44" s="37"/>
+        <v>360</v>
+      </c>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="E45" s="37"/>
+        <v>361</v>
+      </c>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -2887,179 +2866,172 @@
         <v>138</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="E46" s="37"/>
+        <v>342</v>
+      </c>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E47" s="38"/>
+        <v>341</v>
+      </c>
+      <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
+      <c r="A48" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="E49" s="36" t="s">
-        <v>295</v>
+      <c r="E49" s="33" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="E50" s="37"/>
+        <v>261</v>
+      </c>
+      <c r="E50" s="34"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="E51" s="37"/>
+        <v>262</v>
+      </c>
+      <c r="E51" s="34"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="E52" s="37"/>
+        <v>263</v>
+      </c>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E53" s="37"/>
+        <v>264</v>
+      </c>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E54" s="38"/>
+        <v>341</v>
+      </c>
+      <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="40" t="s">
-        <v>278</v>
-      </c>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="42"/>
+      <c r="A55" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="38"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E56" s="36" t="s">
-        <v>298</v>
+        <v>198</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="E57" s="39"/>
+      <c r="E57" s="42"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="E58" s="37"/>
+        <v>267</v>
+      </c>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="E59" s="37"/>
+        <v>342</v>
+      </c>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="14" t="s">
         <v>141</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E60" s="37"/>
+        <v>341</v>
+      </c>
+      <c r="E60" s="34"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>196</v>
+        <v>348</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E61" s="37"/>
+        <v>341</v>
+      </c>
+      <c r="E61" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E2:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E17:E19"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
@@ -3071,19 +3043,26 @@
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A55:E55"/>
+    <mergeCell ref="E2:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png"/>
-    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png"/>
-    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png"/>
-    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png"/>
-    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png"/>
-    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png"/>
-    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png"/>
-    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png"/>
-    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png"/>
-    <hyperlink ref="E16" r:id="rId10"/>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3091,24 +3070,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="97.875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="11"/>
+    <col min="2" max="2" width="97.83203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.95" customHeight="1">
+    <row r="1" spans="1:5" ht="22" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3119,10 +3098,10 @@
         <v>107</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3133,21 +3112,21 @@
         <v>76</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>71</v>
@@ -3159,13 +3138,13 @@
         <v>140</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3173,33 +3152,33 @@
         <v>32</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>302</v>
+        <v>198</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="37"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>376</v>
+        <v>352</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3209,7 +3188,7 @@
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="37"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
@@ -3218,7 +3197,7 @@
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
@@ -3227,7 +3206,7 @@
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -3237,10 +3216,10 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>302</v>
+        <v>342</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3251,9 +3230,9 @@
         <v>77</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E13" s="37"/>
+        <v>198</v>
+      </c>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3263,36 +3242,36 @@
         <v>79</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E14" s="37"/>
+        <v>198</v>
+      </c>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="37"/>
+        <v>198</v>
+      </c>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E16" s="37"/>
+        <v>342</v>
+      </c>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -3301,7 +3280,7 @@
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -3310,7 +3289,7 @@
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -3319,7 +3298,7 @@
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -3328,7 +3307,7 @@
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -3337,7 +3316,7 @@
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="37"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -3346,7 +3325,7 @@
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="37"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -3355,34 +3334,34 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="34" t="s">
-        <v>305</v>
+      <c r="E23" s="40" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="E24" s="40"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>357</v>
-      </c>
       <c r="C25" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3392,8 +3371,8 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="34" t="s">
-        <v>305</v>
+      <c r="E26" s="40" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3403,7 +3382,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="34"/>
+      <c r="E27" s="40"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3412,25 +3391,25 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="34"/>
+      <c r="E28" s="40"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
         <v>172</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>392</v>
-      </c>
-      <c r="E29" s="34"/>
+        <v>391</v>
+      </c>
+      <c r="E29" s="40"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="E30" s="34"/>
+        <v>351</v>
+      </c>
+      <c r="E30" s="40"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3439,8 +3418,8 @@
       <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="37" t="s">
-        <v>377</v>
+      <c r="E31" s="34" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3450,7 +3429,7 @@
       <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3459,7 +3438,7 @@
       <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E33" s="37"/>
+      <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
@@ -3468,17 +3447,17 @@
       <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="37"/>
+      <c r="E34" s="34"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3488,8 +3467,8 @@
       <c r="B36" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="37" t="s">
-        <v>378</v>
+      <c r="E36" s="34" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3499,7 +3478,7 @@
       <c r="B37" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="37"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3508,7 +3487,7 @@
       <c r="B38" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="37"/>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="22" t="s">
@@ -3517,52 +3496,52 @@
       <c r="B39" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="42"/>
+      <c r="A41" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="E42" s="36" t="s">
-        <v>306</v>
+      <c r="E42" s="33" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="37"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -3572,7 +3551,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="37"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -3582,7 +3561,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="37"/>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -3592,7 +3571,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="37"/>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -3602,7 +3581,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="E47" s="37"/>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
@@ -3612,9 +3591,9 @@
         <v>154</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="E48" s="37"/>
+        <v>345</v>
+      </c>
+      <c r="E48" s="34"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="11" t="s">
@@ -3624,42 +3603,42 @@
         <v>153</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="40" t="s">
-        <v>272</v>
-      </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="42"/>
+      <c r="A50" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="38"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="E51" s="36" t="s">
-        <v>373</v>
+      <c r="E51" s="33" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="E52" s="37"/>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -3669,7 +3648,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="E53" s="37"/>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -3679,7 +3658,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="E54" s="37"/>
+      <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
@@ -3689,7 +3668,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="E55" s="37"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="11" t="s">
@@ -3699,9 +3678,9 @@
         <v>157</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="E56" s="37"/>
+        <v>343</v>
+      </c>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
@@ -3711,9 +3690,9 @@
         <v>158</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="E57" s="37"/>
+        <v>344</v>
+      </c>
+      <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3723,7 +3702,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="E58" s="37"/>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3733,7 +3712,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="E59" s="37"/>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="13" t="s">
@@ -3744,10 +3723,10 @@
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E60" s="37" t="s">
-        <v>374</v>
+        <v>197</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3759,19 +3738,19 @@
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E61" s="37"/>
+        <v>197</v>
+      </c>
+      <c r="E61" s="34"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>166</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="E62" s="37"/>
+      <c r="E62" s="34"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="22" t="s">
@@ -3781,8 +3760,8 @@
         <v>169</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="E63" s="37" t="s">
-        <v>375</v>
+      <c r="E63" s="34" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3793,7 +3772,7 @@
         <v>170</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="E64" s="37"/>
+      <c r="E64" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3814,23 +3793,23 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png"/>
-    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png"/>
-    <hyperlink ref="E35" r:id="rId5"/>
-    <hyperlink ref="E40" r:id="rId6"/>
-    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png"/>
-    <hyperlink ref="E49" r:id="rId8"/>
-    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png"/>
-    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png"/>
-    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png"/>
-    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png"/>
-    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png"/>
-    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png"/>
-    <hyperlink ref="E25" r:id="rId15"/>
-    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png"/>
-    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png"/>
+    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E35" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E40" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E49" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E25" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3838,22 +3817,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="28.875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="123.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="26.625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="31.125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" style="11" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="11"/>
+    <col min="7" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3867,207 +3846,207 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>380</v>
+        <v>394</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="E4" s="37"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="37"/>
+        <v>209</v>
+      </c>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>383</v>
+        <v>216</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="E7" s="37"/>
+        <v>217</v>
+      </c>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>380</v>
+        <v>206</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="E11" s="37"/>
+        <v>207</v>
+      </c>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12" s="37"/>
+        <v>204</v>
+      </c>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="E13" s="37"/>
+        <v>364</v>
+      </c>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E14" s="37"/>
+        <v>342</v>
+      </c>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="37"/>
+        <v>198</v>
+      </c>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E16" s="37"/>
+        <v>342</v>
+      </c>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E18" s="37"/>
+        <v>213</v>
+      </c>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>368</v>
-      </c>
       <c r="E19" s="26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
@@ -4076,23 +4055,23 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>382</v>
+        <v>393</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="37"/>
+      <c r="E22" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4104,12 +4083,12 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png"/>
-    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png"/>
-    <hyperlink ref="E19" r:id="rId3"/>
-    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png"/>
-    <hyperlink ref="E9" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4117,21 +4096,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="113.625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="23.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
     <col min="4" max="4" width="14" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="11"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4145,235 +4124,235 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>387</v>
+      <c r="E2" s="33" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E4" s="37"/>
+        <v>341</v>
+      </c>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E5" s="37"/>
+        <v>342</v>
+      </c>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="E6" s="37"/>
+        <v>232</v>
+      </c>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>390</v>
+        <v>251</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" s="38"/>
+        <v>252</v>
+      </c>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="40" t="s">
-        <v>285</v>
-      </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42"/>
+      <c r="A9" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>388</v>
+        <v>198</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>386</v>
+        <v>235</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="E14" s="37"/>
+        <v>236</v>
+      </c>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="E15" s="37"/>
+        <v>237</v>
+      </c>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="38"/>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="40" t="s">
-        <v>286</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
+      <c r="A17" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>249</v>
-      </c>
       <c r="C18" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>391</v>
+        <v>342</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E19" s="37"/>
+        <v>209</v>
+      </c>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="E20" s="37"/>
+        <v>238</v>
+      </c>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="E21" s="37"/>
+        <v>239</v>
+      </c>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="E22" s="37"/>
+        <v>240</v>
+      </c>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="E23" s="38"/>
+        <v>241</v>
+      </c>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -4382,23 +4361,23 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="36" t="s">
-        <v>389</v>
+      <c r="E25" s="33" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="37"/>
+      <c r="E26" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4414,39 +4393,39 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png"/>
-    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png"/>
-    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png"/>
-    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png"/>
-    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png"/>
-    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png"/>
+    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="31.375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="107.625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="107.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="40" style="11" customWidth="1"/>
-    <col min="6" max="6" width="20.375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="36.625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="21.625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="35.125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="21.625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="21.375" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="11"/>
+    <col min="6" max="6" width="20.33203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="35.1640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1">
@@ -4460,7 +4439,7 @@
         <v>106</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -4692,11 +4671,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4765,7 +4744,7 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>31</v>
@@ -4891,7 +4870,7 @@
         <v>80</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>8</v>
@@ -5016,7 +4995,7 @@
         <v>77</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5027,7 +5006,7 @@
         <v>79</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5041,7 +5020,7 @@
         <v>139</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5242,16 +5221,16 @@
         <v>178</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="41"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="42"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="38"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5332,12 +5311,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="40" t="s">
+      <c r="A68" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="41"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="42"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="38"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5442,7 +5421,7 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -5454,7 +5433,7 @@
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -5488,10 +5467,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="40"/>
-      <c r="B83" s="41"/>
-      <c r="C83" s="41"/>
-      <c r="D83" s="42"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
update testdata and add selectTomorrow selectSomeday command
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\STV-Project\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D57C0D-DC78-924D-AB61-10C7BC15A508}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -31,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J T</author>
   </authors>
   <commentList>
-    <comment ref="H10" authorId="0" shapeId="0">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="398">
   <si>
     <t>component</t>
   </si>
@@ -415,7 +416,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -441,7 +442,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -544,7 +545,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -600,7 +601,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -623,7 +624,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -646,7 +647,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -669,7 +670,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -692,7 +693,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -721,7 +722,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -744,7 +745,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -971,7 +972,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -994,7 +995,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1017,7 +1018,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1040,7 +1041,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1114,7 +1115,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1431,7 +1432,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1454,7 +1455,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1477,7 +1478,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1515,7 +1516,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1538,7 +1539,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1556,7 +1557,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1594,7 +1595,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1623,7 +1624,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1649,7 +1650,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1751,7 +1752,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1763,16 +1764,22 @@
     <t>//*[@class='android.widget.TextView' and @text='${NAME}']</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
+  <si>
+    <t>//*[@text='DELETE LIST' and @resource-id='android:id/button1']</t>
+  </si>
+  <si>
+    <t>//*[@text='CANCEL' and @resource-id='android:id/button2']</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1792,14 +1799,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1811,27 +1818,27 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="8" tint="0.59999389629810485"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="4"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1839,7 +1846,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1850,7 +1857,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2026,6 +2033,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2035,6 +2045,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2042,18 +2061,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2073,8 +2080,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2385,21 +2392,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="99.375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="11"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
@@ -2535,13 +2542,13 @@
       <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
@@ -2550,7 +2557,7 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="43" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2561,7 +2568,7 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="44"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
@@ -2588,7 +2595,7 @@
       <c r="D17" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="44" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2599,7 +2606,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2608,16 +2615,16 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="41"/>
+      <c r="E19" s="45"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="37" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -2640,13 +2647,13 @@
       <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
@@ -2687,13 +2694,13 @@
       <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
@@ -2746,13 +2753,13 @@
       <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="39"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
@@ -2815,13 +2822,13 @@
       <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="40" t="s">
         <v>275</v>
       </c>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="45"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
@@ -2887,13 +2894,13 @@
       <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="39"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
@@ -2956,13 +2963,13 @@
       <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="38"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="39"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
@@ -2987,7 +2994,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="E57" s="42"/>
+      <c r="E57" s="36"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3036,6 +3043,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E2:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
@@ -3047,26 +3061,19 @@
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A55:E55"/>
-    <mergeCell ref="E2:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png"/>
-    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png"/>
-    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png"/>
-    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png"/>
-    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png"/>
-    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png"/>
-    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png"/>
-    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png"/>
-    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png"/>
-    <hyperlink ref="E16" r:id="rId10"/>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3074,24 +3081,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="97.875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="11"/>
+    <col min="2" max="2" width="97.83203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.95" customHeight="1">
+    <row r="1" spans="1:5" ht="22" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3338,7 +3345,7 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="44" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3349,7 +3356,7 @@
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
@@ -3375,7 +3382,7 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="44" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3386,7 +3393,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="40"/>
+      <c r="E27" s="44"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3395,7 +3402,7 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" s="44"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
@@ -3404,7 +3411,7 @@
       <c r="B29" s="28" t="s">
         <v>390</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" s="44"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
@@ -3413,7 +3420,7 @@
       <c r="B30" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="44"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3517,13 +3524,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
@@ -3614,13 +3621,13 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="37" t="s">
         <v>271</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="39"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -3797,23 +3804,23 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png"/>
-    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png"/>
-    <hyperlink ref="E35" r:id="rId5"/>
-    <hyperlink ref="E40" r:id="rId6"/>
-    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png"/>
-    <hyperlink ref="E49" r:id="rId8"/>
-    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png"/>
-    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png"/>
-    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png"/>
-    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png"/>
-    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png"/>
-    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png"/>
-    <hyperlink ref="E25" r:id="rId15"/>
-    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png"/>
-    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png"/>
+    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E35" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E40" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E49" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E25" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3821,22 +3828,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="28.875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="123.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="26.625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="31.125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" style="11" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="11"/>
+    <col min="7" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4087,12 +4094,12 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png"/>
-    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png"/>
-    <hyperlink ref="E19" r:id="rId3"/>
-    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png"/>
-    <hyperlink ref="E9" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4100,21 +4107,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="113.625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="23.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
     <col min="4" max="4" width="14" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="11"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4208,13 +4215,13 @@
       <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
@@ -4287,13 +4294,13 @@
       <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="37" t="s">
         <v>285</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -4368,7 +4375,7 @@
         <v>333</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>73</v>
+        <v>396</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>387</v>
@@ -4379,7 +4386,7 @@
         <v>334</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>74</v>
+        <v>397</v>
       </c>
       <c r="E26" s="34"/>
     </row>
@@ -4397,39 +4404,39 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png"/>
-    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png"/>
-    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png"/>
-    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png"/>
-    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png"/>
-    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png"/>
+    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="31.375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="107.625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="107.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="40" style="11" customWidth="1"/>
-    <col min="6" max="6" width="20.375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="36.625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="21.625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="35.125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="21.625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="21.375" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="11"/>
+    <col min="6" max="6" width="20.33203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="35.1640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1">
@@ -4675,11 +4682,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4802,11 +4809,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -5229,12 +5236,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="38"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="39"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5315,12 +5322,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="36" t="s">
+      <c r="A68" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="38"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="39"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5471,10 +5478,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="36"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="38"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Add edge coverage scripts
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DDF3FB-6DD8-0F40-A473-6ED98F0B7523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A443EB-C264-F74C-BCEB-7330E6A93C68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8120" yWindow="460" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="All" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TaskList!$A$1:$E$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ViewTask!$A$1:$A$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="401">
   <si>
     <t>component</t>
   </si>
@@ -1769,6 +1770,15 @@
   </si>
   <si>
     <t>//*[@text='CANCEL' and @resource-id='android:id/button2']</t>
+  </si>
+  <si>
+    <t>Send to</t>
+  </si>
+  <si>
+    <t>send_to_see_all</t>
+  </si>
+  <si>
+    <t>send_to_create_task</t>
   </si>
 </sst>
 </file>
@@ -2033,9 +2043,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2045,6 +2052,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2052,15 +2071,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2395,8 +2405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -2542,13 +2552,13 @@
       <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
@@ -2557,7 +2567,7 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="39" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2568,7 +2578,7 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="44"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
@@ -2595,7 +2605,7 @@
       <c r="D17" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="40" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2606,7 +2616,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="44"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2615,16 +2625,16 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="45"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -2647,13 +2657,13 @@
       <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
@@ -2694,13 +2704,13 @@
       <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
@@ -2753,13 +2763,13 @@
       <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="38"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
@@ -2822,13 +2832,13 @@
       <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="43" t="s">
         <v>275</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="42"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="45"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
@@ -2894,13 +2904,13 @@
       <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
@@ -2963,13 +2973,13 @@
       <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="39"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="38"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
@@ -2994,7 +3004,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="E57" s="36"/>
+      <c r="E57" s="42"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3043,13 +3053,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E2:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E17:E19"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
@@ -3061,6 +3064,13 @@
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A55:E55"/>
+    <mergeCell ref="E2:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
@@ -3084,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -3345,7 +3355,7 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="40" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3356,7 +3366,7 @@
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="44"/>
+      <c r="E24" s="40"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
@@ -3382,7 +3392,7 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="40" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3393,7 +3403,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="44"/>
+      <c r="E27" s="40"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3402,7 +3412,7 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="44"/>
+      <c r="E28" s="40"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
@@ -3411,7 +3421,7 @@
       <c r="B29" s="28" t="s">
         <v>390</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="40"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
@@ -3420,7 +3430,7 @@
       <c r="B30" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="E30" s="44"/>
+      <c r="E30" s="40"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3524,13 +3534,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
@@ -3621,13 +3631,13 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="39"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="38"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -3829,10 +3839,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -4084,8 +4094,34 @@
       </c>
       <c r="E22" s="34"/>
     </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="50"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A23:E23"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="A20:E20"/>
@@ -4215,13 +4251,13 @@
       <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
@@ -4294,13 +4330,13 @@
       <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -4683,11 +4719,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4810,11 +4846,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -5237,12 +5273,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="39"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="38"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5323,12 +5359,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="39"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="38"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5479,10 +5515,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="37"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="39"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
modify category coverage scripts, update test data, modify scroll duration, add view task script
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0FD24D-CB74-FE48-8211-F1DA0CEB376A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F19B2B1-248C-F448-8FFD-277A8306C3A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="660" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="All" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TaskList!$A$1:$E$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ViewTask!$A$1:$A$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -76,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="398">
   <si>
     <t>component</t>
   </si>
@@ -1364,9 +1363,6 @@
     <t>menu_send_to_btn</t>
   </si>
   <si>
-    <t>menu_create_teask_btn</t>
-  </si>
-  <si>
     <t>menu_see_all_btn</t>
   </si>
   <si>
@@ -1772,19 +1768,7 @@
     <t>//*[@text='CANCEL' and @resource-id='android:id/button2']</t>
   </si>
   <si>
-    <t>Send to</t>
-  </si>
-  <si>
-    <t>send_to_see_all</t>
-  </si>
-  <si>
-    <t>send_to_create_task</t>
-  </si>
-  <si>
-    <t>pager</t>
-  </si>
-  <si>
-    <t>//*[@class='android.support.v4.view.ViewPager']</t>
+    <t>menu_create_task_btn</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +1954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2040,9 +2024,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2050,9 +2031,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2064,6 +2042,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2071,15 +2061,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2412,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -2428,7 +2409,7 @@
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1">
+    <row r="1" spans="1:6" ht="21" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2445,36 +2426,36 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="33" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="35"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="35"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="34"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2482,9 +2463,9 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="35"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="34"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -2492,9 +2473,9 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="35"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -2502,9 +2483,9 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="35"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
@@ -2512,9 +2493,9 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="35"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
         <v>272</v>
       </c>
@@ -2522,21 +2503,21 @@
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="35"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E10" s="35"/>
-    </row>
-    <row r="11" spans="1:5">
+        <v>340</v>
+      </c>
+      <c r="E10" s="34"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -2544,565 +2525,555 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="E11" s="35"/>
-    </row>
-    <row r="12" spans="1:5">
+        <v>341</v>
+      </c>
+      <c r="E11" s="34"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="E13" s="33"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>369</v>
+      </c>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="45"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>370</v>
-      </c>
-      <c r="F17" s="31"/>
-    </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E18" s="45" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>73</v>
+      </c>
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="41"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="45"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="46"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="E21" s="33" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
         <v>333</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="11" t="s">
-        <v>334</v>
-      </c>
-      <c r="B23" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="36"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="38" t="s">
+      <c r="E22" s="35"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="40"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="14" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>222</v>
+      </c>
+      <c r="E25" s="34"/>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="E26" s="35"/>
-    </row>
-    <row r="27" spans="1:6">
+        <v>223</v>
+      </c>
+      <c r="E26" s="34"/>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E27" s="35"/>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E28" s="36"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="38" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="40"/>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="E30" s="34" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>254</v>
+      </c>
+      <c r="E30" s="34"/>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E31" s="35"/>
-    </row>
-    <row r="32" spans="1:6">
+        <v>255</v>
+      </c>
+      <c r="E31" s="34"/>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E32" s="35"/>
+        <v>256</v>
+      </c>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
-        <v>315</v>
+        <v>141</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>256</v>
+        <v>346</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>340</v>
       </c>
       <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E34" s="36"/>
+      <c r="A34" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="38"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="38" t="s">
-        <v>274</v>
-      </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="40"/>
+      <c r="A35" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="E35" s="33" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="23" t="s">
-        <v>316</v>
+      <c r="A36" s="11" t="s">
+        <v>312</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="E36" s="34" t="s">
-        <v>292</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="E36" s="34"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="E37" s="35"/>
+        <v>254</v>
+      </c>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="11" t="s">
-        <v>313</v>
+      <c r="A38" s="13" t="s">
+        <v>315</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E38" s="35"/>
+        <v>256</v>
+      </c>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="13" t="s">
-        <v>315</v>
+      <c r="A39" s="11" t="s">
+        <v>317</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E39" s="35"/>
+        <v>258</v>
+      </c>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
-        <v>317</v>
+        <v>141</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>258</v>
+        <v>346</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>340</v>
       </c>
       <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E41" s="36"/>
+      <c r="A41" s="43" t="s">
+        <v>275</v>
+      </c>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="45"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="43"/>
+      <c r="A42" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="E42" s="33" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="23" t="s">
-        <v>318</v>
+      <c r="A43" s="11" t="s">
+        <v>319</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="E43" s="34" t="s">
-        <v>293</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="E44" s="35"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="E45" s="35"/>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="E46" s="35"/>
+        <v>21</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>342</v>
+        <v>141</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>340</v>
       </c>
       <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E48" s="36"/>
+      <c r="A48" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="38" t="s">
-        <v>276</v>
-      </c>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="40"/>
+      <c r="A49" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="E49" s="33" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="23" t="s">
-        <v>322</v>
+      <c r="A50" s="11" t="s">
+        <v>323</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="C50" s="7"/>
-      <c r="E50" s="34" t="s">
-        <v>294</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="E50" s="34"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="E51" s="35"/>
+        <v>262</v>
+      </c>
+      <c r="E51" s="34"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="E52" s="35"/>
+        <v>263</v>
+      </c>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="E53" s="35"/>
+        <v>264</v>
+      </c>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
-        <v>326</v>
+        <v>141</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>264</v>
+        <v>346</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>340</v>
       </c>
       <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E55" s="36"/>
+      <c r="A55" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="38"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="40"/>
+      <c r="A56" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>265</v>
+      <c r="A57" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>297</v>
-      </c>
+      <c r="E57" s="42"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C58" s="7"/>
-      <c r="E58" s="37"/>
+        <v>360</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="E59" s="34"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="E59" s="35"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="E60" s="35"/>
+      <c r="C60" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="E60" s="34"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>362</v>
+      <c r="A61" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>394</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E61" s="35"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="E62" s="35"/>
+        <v>340</v>
+      </c>
+      <c r="E61" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="E49:E54"/>
+    <mergeCell ref="E56:E61"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A55:E55"/>
     <mergeCell ref="E2:E12"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="E50:E55"/>
-    <mergeCell ref="E57:E62"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="E30:E34"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="E36:E41"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E22:E23" r:id="rId1" display="ConfirmDelete.png" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E25:E28" r:id="rId2" display="TaskListMenu.png" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E30:E34" r:id="rId3" display="TasksDue.png" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E36:E41" r:id="rId4" display="TasksStarting.png" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E43:E48" r:id="rId5" display="TasksPriority.png" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E50:E55" r:id="rId6" display="TaskProgress.png" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E57:E62" r:id="rId7" display="Search.png" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E18:E20" r:id="rId9" display="QuickAdd.png" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3113,8 +3084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A20" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -3151,7 +3122,7 @@
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="46" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3160,9 +3131,9 @@
         <v>218</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="E3" s="48"/>
+        <v>367</v>
+      </c>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
@@ -3171,17 +3142,17 @@
       <c r="B4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="47"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="22" t="s">
         <v>140</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>303</v>
@@ -3192,12 +3163,12 @@
         <v>32</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3208,17 +3179,17 @@
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>351</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>374</v>
+        <v>350</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3228,7 +3199,7 @@
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
@@ -3237,7 +3208,7 @@
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
@@ -3246,7 +3217,7 @@
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -3256,9 +3227,9 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E12" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3272,7 +3243,7 @@
       <c r="D13" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3284,34 +3255,34 @@
       <c r="D14" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E16" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -3320,7 +3291,7 @@
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -3329,7 +3300,7 @@
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -3338,7 +3309,7 @@
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -3347,7 +3318,7 @@
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -3356,7 +3327,7 @@
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -3365,7 +3336,7 @@
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -3374,7 +3345,7 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="40" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3385,23 +3356,23 @@
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="45"/>
+      <c r="E24" s="40"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>355</v>
-      </c>
       <c r="C25" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3411,7 +3382,7 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="45" t="s">
+      <c r="E26" s="40" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3422,7 +3393,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="45"/>
+      <c r="E27" s="40"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3431,25 +3402,25 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="45"/>
+      <c r="E28" s="40"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
         <v>172</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>390</v>
-      </c>
-      <c r="E29" s="45"/>
+        <v>389</v>
+      </c>
+      <c r="E29" s="40"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
         <v>298</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="E30" s="45"/>
+        <v>349</v>
+      </c>
+      <c r="E30" s="40"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3458,8 +3429,8 @@
       <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="35" t="s">
-        <v>375</v>
+      <c r="E31" s="34" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3469,7 +3440,7 @@
       <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="35"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3478,7 +3449,7 @@
       <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E33" s="35"/>
+      <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
@@ -3487,14 +3458,14 @@
       <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="35"/>
+      <c r="E34" s="34"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
         <v>299</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E35" s="26" t="s">
         <v>304</v>
@@ -3507,8 +3478,8 @@
       <c r="B36" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="35" t="s">
-        <v>376</v>
+      <c r="E36" s="34" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3518,7 +3489,7 @@
       <c r="B37" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="35"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3527,7 +3498,7 @@
       <c r="B38" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="22" t="s">
@@ -3536,14 +3507,14 @@
       <c r="B39" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="35"/>
+      <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>198</v>
@@ -3553,13 +3524,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="40"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
@@ -3569,7 +3540,7 @@
         <v>73</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="E42" s="34" t="s">
+      <c r="E42" s="33" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3581,7 +3552,7 @@
         <v>74</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="35"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -3591,7 +3562,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="35"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -3601,7 +3572,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="35"/>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -3611,7 +3582,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="35"/>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -3621,7 +3592,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="E47" s="35"/>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
@@ -3631,9 +3602,9 @@
         <v>154</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="E48" s="35"/>
+        <v>344</v>
+      </c>
+      <c r="E48" s="34"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="11" t="s">
@@ -3643,20 +3614,20 @@
         <v>153</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E49" s="26" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="40"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="38"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -3666,8 +3637,8 @@
         <v>73</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="E51" s="34" t="s">
-        <v>371</v>
+      <c r="E51" s="33" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3678,7 +3649,7 @@
         <v>74</v>
       </c>
       <c r="C52" s="15"/>
-      <c r="E52" s="35"/>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -3688,7 +3659,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="E53" s="35"/>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -3698,7 +3669,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="E54" s="35"/>
+      <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
@@ -3708,7 +3679,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="E55" s="35"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="11" t="s">
@@ -3718,9 +3689,9 @@
         <v>157</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="E56" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
@@ -3730,9 +3701,9 @@
         <v>158</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="E57" s="35"/>
+        <v>343</v>
+      </c>
+      <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3742,7 +3713,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="E58" s="35"/>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3752,7 +3723,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="E59" s="35"/>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="13" t="s">
@@ -3765,8 +3736,8 @@
       <c r="D60" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E60" s="35" t="s">
-        <v>372</v>
+      <c r="E60" s="34" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3780,7 +3751,7 @@
       <c r="D61" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E61" s="35"/>
+      <c r="E61" s="34"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
@@ -3790,7 +3761,7 @@
         <v>166</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="E62" s="35"/>
+      <c r="E62" s="34"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="22" t="s">
@@ -3800,8 +3771,8 @@
         <v>169</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="E63" s="35" t="s">
-        <v>373</v>
+      <c r="E63" s="34" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3812,7 +3783,7 @@
         <v>170</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="E64" s="35"/>
+      <c r="E64" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3858,10 +3829,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -3897,10 +3868,10 @@
         <v>199</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>378</v>
+        <v>392</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3910,7 +3881,7 @@
       <c r="B3" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
@@ -3919,7 +3890,7 @@
       <c r="B4" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
@@ -3928,7 +3899,7 @@
       <c r="B5" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
@@ -3937,8 +3908,8 @@
       <c r="B6" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>381</v>
+      <c r="E6" s="34" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3948,49 +3919,49 @@
       <c r="B7" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>329</v>
+        <v>397</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>219</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>378</v>
+      <c r="E10" s="34" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
@@ -3999,16 +3970,16 @@
       <c r="B12" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
         <v>208</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="E13" s="35"/>
+        <v>362</v>
+      </c>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -4018,9 +3989,9 @@
         <v>228</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E14" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
@@ -4030,12 +4001,12 @@
         <v>229</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="30" t="s">
@@ -4045,9 +4016,9 @@
         <v>230</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E16" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
@@ -4056,7 +4027,7 @@
       <c r="B17" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
@@ -4065,82 +4036,56 @@
       <c r="B18" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
         <v>215</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>366</v>
-      </c>
       <c r="E19" s="26" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="50"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>380</v>
+        <v>391</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="35"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="49" t="s">
-        <v>398</v>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="51"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="20" t="s">
-        <v>400</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>219</v>
-      </c>
+      <c r="E22" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A23:E23"/>
+  <mergeCells count="5">
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="A20:E20"/>
@@ -4165,7 +4110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4203,8 +4148,8 @@
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>385</v>
+      <c r="E2" s="33" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4214,7 +4159,7 @@
       <c r="B3" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
@@ -4224,21 +4169,21 @@
         <v>227</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="E4" s="35"/>
+        <v>340</v>
+      </c>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
         <v>231</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E5" s="35"/>
+        <v>341</v>
+      </c>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
@@ -4247,7 +4192,7 @@
       <c r="B6" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="E6" s="35"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
@@ -4256,8 +4201,8 @@
       <c r="B7" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>388</v>
+      <c r="E7" s="34" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4267,16 +4212,16 @@
       <c r="B8" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
@@ -4288,74 +4233,74 @@
       <c r="D10" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>386</v>
+      <c r="E10" s="33" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="E13" s="35" t="s">
-        <v>384</v>
+      <c r="E13" s="34" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -4365,10 +4310,10 @@
         <v>248</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>389</v>
+        <v>341</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4378,7 +4323,7 @@
       <c r="B19" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -4387,7 +4332,7 @@
       <c r="B20" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -4396,7 +4341,7 @@
       <c r="B21" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -4405,7 +4350,7 @@
       <c r="B22" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -4414,36 +4359,36 @@
       <c r="B23" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>387</v>
+        <v>395</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="E26" s="35"/>
+        <v>396</v>
+      </c>
+      <c r="E26" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4738,11 +4683,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4865,11 +4810,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -5292,12 +5237,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="38" t="s">
+      <c r="A59" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="40"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="38"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5378,12 +5323,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="38" t="s">
+      <c r="A68" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="40"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="38"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5534,10 +5479,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="38"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="40"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
fix fuck bug in testdata
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\STV-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F19B2B1-248C-F448-8FFD-277A8306C3A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>J T</author>
   </authors>
   <commentList>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="H10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="401">
   <si>
     <t>component</t>
   </si>
@@ -416,7 +415,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -442,7 +441,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -545,7 +544,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -601,7 +600,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -624,7 +623,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -647,7 +646,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -670,7 +669,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -693,7 +692,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -722,7 +721,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -745,7 +744,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -972,7 +971,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -995,7 +994,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1018,7 +1017,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1041,7 +1040,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1115,7 +1114,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1249,9 +1248,6 @@
     <t>TaskListMenu.png</t>
   </si>
   <si>
-    <t>TasksDue.png</t>
-  </si>
-  <si>
     <t>TasksStarting.png</t>
   </si>
   <si>
@@ -1361,9 +1357,6 @@
   </si>
   <si>
     <t>menu_send_to_btn</t>
-  </si>
-  <si>
-    <t>menu_see_all_btn</t>
   </si>
   <si>
     <t>+1day_btn</t>
@@ -1429,7 +1422,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1452,7 +1445,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1475,7 +1468,7 @@
       <rPr>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1513,7 +1506,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1536,7 +1529,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1554,7 +1547,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1592,7 +1585,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1621,7 +1614,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1647,7 +1640,7 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1749,7 +1742,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1768,18 +1761,39 @@
     <t>//*[@text='CANCEL' and @resource-id='android:id/button2']</t>
   </si>
   <si>
+    <t>menu_see_all_btn</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
     <t>menu_create_task_btn</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>task</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>TasksDue.png</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>pager</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>//*[@class='android.support.v4.view.ViewPager']</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1799,14 +1813,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1818,27 +1832,27 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="8" tint="0.59999389629810485"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="4"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1846,7 +1860,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1857,7 +1871,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2033,6 +2047,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2042,6 +2059,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2049,18 +2075,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2080,8 +2094,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2392,21 +2406,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="99.375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.625" style="11" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1">
@@ -2434,7 +2448,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2510,10 +2524,10 @@
         <v>140</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E10" s="34"/>
     </row>
@@ -2525,7 +2539,7 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E11" s="34"/>
     </row>
@@ -2534,21 +2548,21 @@
         <v>141</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
@@ -2557,7 +2571,7 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="43" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2568,20 +2582,20 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="44"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F16" s="31"/>
     </row>
@@ -2595,7 +2609,7 @@
       <c r="D17" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="44" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2606,7 +2620,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2615,20 +2629,20 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="41"/>
+      <c r="E19" s="45"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="37" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
@@ -2639,7 +2653,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
@@ -2647,13 +2661,13 @@
       <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
@@ -2694,28 +2708,28 @@
       <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>253</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>291</v>
+        <v>398</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>254</v>
@@ -2724,7 +2738,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>255</v>
@@ -2733,7 +2747,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>256</v>
@@ -2742,318 +2756,316 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
-        <v>141</v>
+        <v>399</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="E33" s="35"/>
+        <v>400</v>
+      </c>
+      <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E34" s="35"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="23" t="s">
-        <v>316</v>
-      </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="39"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="E35" s="33" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="E36" s="34"/>
+      <c r="C36" s="7"/>
+      <c r="E36" s="33" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E37" s="34"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E37" s="34"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="B38" s="11" t="s">
+      <c r="E38" s="34"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>256</v>
-      </c>
-      <c r="E38" s="34"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>258</v>
       </c>
       <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="E40" s="34"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="E40" s="35"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="43" t="s">
+      <c r="B41" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E41" s="35"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="40" t="s">
         <v>275</v>
       </c>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="45"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="23" t="s">
-        <v>318</v>
-      </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="42"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="E42" s="33" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="E43" s="34"/>
+      <c r="C43" s="7"/>
+      <c r="E43" s="33" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>341</v>
+        <v>320</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>357</v>
       </c>
       <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="E47" s="34"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B47" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="E47" s="35"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="36" t="s">
+      <c r="B48" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E48" s="35"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="38"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="23" t="s">
-        <v>322</v>
-      </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="39"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="E49" s="33" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="E50" s="34"/>
+      <c r="C50" s="7"/>
+      <c r="E50" s="33" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E51" s="34"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E54" s="34"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="E54" s="35"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="36" t="s">
+      <c r="B55" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E55" s="35"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="38"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="23" t="s">
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="39"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B57" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="11" t="s">
+      <c r="C57" s="7"/>
+      <c r="D57" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E56" s="33" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="11" t="s">
+      <c r="E57" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="7"/>
-      <c r="E57" s="42"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="E58" s="34"/>
+        <v>295</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="7"/>
+      <c r="E58" s="36"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="B59" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E59" s="34"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B60" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C59" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="E59" s="34"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="14" t="s">
+      <c r="C60" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="E60" s="34"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="E60" s="34"/>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="11" t="s">
+      <c r="B61" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E61" s="34"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="E61" s="34"/>
+      <c r="B62" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E62" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="E49:E54"/>
-    <mergeCell ref="E56:E61"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A55:E55"/>
     <mergeCell ref="E2:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A20:E20"/>
@@ -3061,19 +3073,30 @@
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="E50:E55"/>
+    <mergeCell ref="E57:E62"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="E36:E41"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A56:E56"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png"/>
+    <hyperlink ref="E29:E34" r:id="rId3" display="TasksDue.png"/>
+    <hyperlink ref="E36:E41" r:id="rId4" display="TasksStarting.png"/>
+    <hyperlink ref="E43:E48" r:id="rId5" display="TasksPriority.png"/>
+    <hyperlink ref="E50:E55" r:id="rId6" display="TaskProgress.png"/>
+    <hyperlink ref="E57:E62" r:id="rId7" display="Search.png"/>
+    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png"/>
+    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png"/>
+    <hyperlink ref="E16" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3081,24 +3104,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A20" zoomScale="108" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="97.83203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="11"/>
+    <col min="2" max="2" width="97.875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.625" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" customHeight="1">
+    <row r="1" spans="1:5" ht="21.95" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3123,7 +3146,7 @@
         <v>76</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3131,13 +3154,13 @@
         <v>218</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>71</v>
@@ -3149,13 +3172,13 @@
         <v>140</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3163,13 +3186,13 @@
         <v>32</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>198</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3186,10 +3209,10 @@
         <v>142</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3227,10 +3250,10 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3262,10 +3285,10 @@
         <v>39</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>198</v>
@@ -3277,10 +3300,10 @@
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E16" s="34"/>
     </row>
@@ -3345,34 +3368,34 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="40" t="s">
-        <v>304</v>
+      <c r="E23" s="44" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>356</v>
-      </c>
       <c r="E25" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3382,8 +3405,8 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="40" t="s">
-        <v>304</v>
+      <c r="E26" s="44" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3393,7 +3416,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="40"/>
+      <c r="E27" s="44"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3402,25 +3425,25 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" s="44"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
         <v>172</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>389</v>
-      </c>
-      <c r="E29" s="40"/>
+        <v>387</v>
+      </c>
+      <c r="E29" s="44"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="E30" s="40"/>
+        <v>347</v>
+      </c>
+      <c r="E30" s="44"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3430,7 +3453,7 @@
         <v>184</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3462,13 +3485,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3479,7 +3502,7 @@
         <v>195</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3514,39 +3537,39 @@
         <v>174</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>198</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="15"/>
       <c r="E42" s="33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>74</v>
@@ -3602,7 +3625,7 @@
         <v>154</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E48" s="34"/>
     </row>
@@ -3614,36 +3637,36 @@
         <v>153</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="37" t="s">
         <v>271</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="39"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C51" s="15"/>
       <c r="E51" s="33" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>74</v>
@@ -3689,7 +3712,7 @@
         <v>157</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E56" s="34"/>
     </row>
@@ -3701,7 +3724,7 @@
         <v>158</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E57" s="34"/>
     </row>
@@ -3737,7 +3760,7 @@
         <v>197</v>
       </c>
       <c r="E60" s="34" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3755,7 +3778,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>166</v>
@@ -3772,7 +3795,7 @@
       </c>
       <c r="C63" s="15"/>
       <c r="E63" s="34" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3804,23 +3827,23 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="E35" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="E40" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="E49" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="E25" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png"/>
+    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png"/>
+    <hyperlink ref="E35" r:id="rId5"/>
+    <hyperlink ref="E40" r:id="rId6"/>
+    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png"/>
+    <hyperlink ref="E49" r:id="rId8"/>
+    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png"/>
+    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png"/>
+    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png"/>
+    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png"/>
+    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png"/>
+    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png"/>
+    <hyperlink ref="E25" r:id="rId15"/>
+    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png"/>
+    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3828,22 +3851,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="28.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="123.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="31.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="31.125" style="11" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="11"/>
+    <col min="7" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3868,10 +3891,10 @@
         <v>199</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3903,18 +3926,18 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>216</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>217</v>
@@ -3923,40 +3946,40 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>219</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>329</v>
+        <v>395</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>206</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>207</v>
@@ -3977,7 +4000,7 @@
         <v>208</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E13" s="34"/>
     </row>
@@ -3989,7 +4012,7 @@
         <v>228</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E14" s="34"/>
     </row>
@@ -4001,7 +4024,7 @@
         <v>229</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>198</v>
@@ -4016,7 +4039,7 @@
         <v>230</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E16" s="34"/>
     </row>
@@ -4043,16 +4066,16 @@
         <v>215</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>365</v>
-      </c>
       <c r="E19" s="26" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -4066,18 +4089,18 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
@@ -4094,12 +4117,12 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="E19" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png"/>
+    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png"/>
+    <hyperlink ref="E19" r:id="rId3"/>
+    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png"/>
+    <hyperlink ref="E9" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4107,21 +4130,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="27.625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="113.625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="23.375" style="11" customWidth="1"/>
     <col min="4" max="4" width="14" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="21.625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4149,7 +4172,7 @@
         <v>67</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4169,7 +4192,7 @@
         <v>227</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E4" s="34"/>
     </row>
@@ -4178,10 +4201,10 @@
         <v>231</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E5" s="34"/>
     </row>
@@ -4202,7 +4225,7 @@
         <v>251</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4215,13 +4238,13 @@
       <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
@@ -4234,12 +4257,12 @@
         <v>198</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>73</v>
@@ -4248,7 +4271,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>74</v>
@@ -4257,18 +4280,18 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>235</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>236</v>
@@ -4277,7 +4300,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>237</v>
@@ -4286,7 +4309,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>74</v>
@@ -4294,13 +4317,13 @@
       <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="37" t="s">
         <v>285</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -4310,10 +4333,10 @@
         <v>248</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4372,21 +4395,21 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E26" s="34"/>
     </row>
@@ -4404,12 +4427,12 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png"/>
+    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png"/>
+    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png"/>
+    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png"/>
+    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png"/>
+    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4417,27 +4440,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="107.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="31.375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="107.625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20.125" style="11" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="40" style="11" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="35.1640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="11"/>
+    <col min="6" max="6" width="20.375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="36.625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="35.125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="21.625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="21.375" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1">
@@ -4683,11 +4706,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4810,11 +4833,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -5237,12 +5260,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="38"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="39"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5323,12 +5346,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="36" t="s">
+      <c r="A68" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="38"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="39"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5479,10 +5502,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="36"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="38"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
complete input space partition tesst
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\STV-Project\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\STV-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="402">
   <si>
     <t>component</t>
   </si>
@@ -1784,12 +1784,54 @@
     <t>//*[@class='android.support.v4.view.ViewPager']</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//*[@class='android.widget.ScrollView']</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//*[@class='android.widget.TextView' and @text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${YEAR}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']</t>
+    </r>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1873,6 +1915,14 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -2047,9 +2097,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2059,6 +2106,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2066,15 +2125,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2409,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
@@ -2556,13 +2606,13 @@
       <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
@@ -2571,7 +2621,7 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="39" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2582,7 +2632,7 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="44"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
@@ -2609,7 +2659,7 @@
       <c r="D17" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="40" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2620,7 +2670,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="44"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2629,16 +2679,16 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="45"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -2661,13 +2711,13 @@
       <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
@@ -2708,13 +2758,13 @@
       <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
@@ -2776,13 +2826,13 @@
       <c r="E34" s="35"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="38"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="23" t="s">
@@ -2845,13 +2895,13 @@
       <c r="E41" s="35"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="43" t="s">
         <v>275</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="42"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="45"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="23" t="s">
@@ -2917,13 +2967,13 @@
       <c r="E48" s="35"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="39"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="38"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="23" t="s">
@@ -2986,13 +3036,13 @@
       <c r="E55" s="35"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="39"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="38"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="23" t="s">
@@ -3017,7 +3067,7 @@
         <v>67</v>
       </c>
       <c r="C58" s="7"/>
-      <c r="E58" s="36"/>
+      <c r="E58" s="42"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3066,13 +3116,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E2:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E17:E19"/>
     <mergeCell ref="E43:E48"/>
     <mergeCell ref="E50:E55"/>
     <mergeCell ref="E57:E62"/>
@@ -3084,6 +3127,13 @@
     <mergeCell ref="E36:E41"/>
     <mergeCell ref="A49:E49"/>
     <mergeCell ref="A56:E56"/>
+    <mergeCell ref="E2:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
@@ -3107,8 +3157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="108" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5"/>
@@ -3368,7 +3418,7 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="40" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3379,7 +3429,7 @@
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="44"/>
+      <c r="E24" s="40"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
@@ -3405,7 +3455,7 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="40" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3416,7 +3466,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="44"/>
+      <c r="E27" s="40"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3425,7 +3475,7 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="44"/>
+      <c r="E28" s="40"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
@@ -3434,7 +3484,7 @@
       <c r="B29" s="28" t="s">
         <v>387</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="40"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
@@ -3443,7 +3493,7 @@
       <c r="B30" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="E30" s="44"/>
+      <c r="E30" s="40"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3547,13 +3597,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
@@ -3634,7 +3684,7 @@
         <v>128</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>153</v>
+        <v>401</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>343</v>
@@ -3644,13 +3694,13 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="39"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="38"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
@@ -4238,13 +4288,13 @@
       <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
@@ -4317,13 +4367,13 @@
       <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -4706,11 +4756,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4833,11 +4883,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -5260,12 +5310,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="39"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="38"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5346,12 +5396,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="39"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="38"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5502,10 +5552,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="37"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="39"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>